<commit_message>
ComX means different things in different regions
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\VEDA_Models\Demo_Adv_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9683EE7-A9D7-48B5-AA5B-780DD970506A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA02264D-595B-45BB-A664-007BBAFCAC3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="570" windowWidth="25080" windowHeight="15030" tabRatio="853" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="853" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region-Time Slices" sheetId="16" r:id="rId1"/>
@@ -21,9 +21,10 @@
     <sheet name="TimeSlices" sheetId="22" r:id="rId6"/>
     <sheet name="Defaults" sheetId="21" r:id="rId7"/>
     <sheet name="Commodity Group" sheetId="15" r:id="rId8"/>
+    <sheet name="Commodities" sheetId="24" r:id="rId9"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId10"/>
   </externalReferences>
   <definedNames>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
@@ -260,7 +261,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="207">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -863,6 +864,24 @@
   </si>
   <si>
     <t>*ELC</t>
+  </si>
+  <si>
+    <t>AT,DE,FR,ES,IT,BE,NL,UK</t>
+  </si>
+  <si>
+    <t>REG1,REG2</t>
+  </si>
+  <si>
+    <t>ComX</t>
+  </si>
+  <si>
+    <t>SEASON</t>
+  </si>
+  <si>
+    <t>commodity x in elc regions</t>
+  </si>
+  <si>
+    <t>commodity x in non-elc regions</t>
   </si>
 </sst>
 </file>
@@ -3831,10 +3850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:N38"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3846,6 +3865,16 @@
     <col min="8" max="8" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N2" t="s">
+        <v>202</v>
+      </c>
+    </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="6"/>
       <c r="B3" s="1" t="s">
@@ -5997,10 +6026,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="B1:J34"/>
+  <dimension ref="B1:I9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6017,7 +6046,7 @@
     <col min="10" max="11" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -6026,7 +6055,7 @@
       <c r="G1" s="6"/>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="2:10" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B2" s="7" t="s">
         <v>36</v>
       </c>
@@ -6037,7 +6066,7 @@
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="4" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
@@ -6046,12 +6075,12 @@
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
@@ -6077,7 +6106,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>37</v>
       </c>
@@ -6091,7 +6120,7 @@
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>195</v>
       </c>
@@ -6108,7 +6137,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>199</v>
       </c>
@@ -6123,425 +6152,6 @@
       </c>
       <c r="I9" t="s">
         <v>197</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="127" t="s">
-        <v>166</v>
-      </c>
-      <c r="C12" s="127"/>
-      <c r="D12" s="127"/>
-      <c r="E12" s="127"/>
-      <c r="F12" s="127"/>
-      <c r="G12" s="127"/>
-      <c r="H12" s="127"/>
-      <c r="I12" s="127"/>
-      <c r="J12" s="127"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="127" t="s">
-        <v>167</v>
-      </c>
-      <c r="C13" s="127" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="127" t="s">
-        <v>168</v>
-      </c>
-      <c r="E13" s="127" t="s">
-        <v>169</v>
-      </c>
-      <c r="F13" s="127" t="s">
-        <v>170</v>
-      </c>
-      <c r="G13" s="127" t="s">
-        <v>21</v>
-      </c>
-      <c r="H13" s="127" t="s">
-        <v>171</v>
-      </c>
-      <c r="I13" s="127" t="s">
-        <v>131</v>
-      </c>
-      <c r="J13" s="127" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="127" t="s">
-        <v>134</v>
-      </c>
-      <c r="C14" s="127"/>
-      <c r="D14" s="127" t="s">
-        <v>132</v>
-      </c>
-      <c r="E14" s="127" t="s">
-        <v>133</v>
-      </c>
-      <c r="F14" s="127" t="s">
-        <v>52</v>
-      </c>
-      <c r="G14" s="127"/>
-      <c r="H14" s="127"/>
-      <c r="I14" s="127"/>
-      <c r="J14" s="127"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="127" t="s">
-        <v>134</v>
-      </c>
-      <c r="C15" s="127"/>
-      <c r="D15" s="127" t="s">
-        <v>135</v>
-      </c>
-      <c r="E15" s="127" t="s">
-        <v>136</v>
-      </c>
-      <c r="F15" s="127" t="s">
-        <v>52</v>
-      </c>
-      <c r="G15" s="127"/>
-      <c r="H15" s="127"/>
-      <c r="I15" s="127"/>
-      <c r="J15" s="127"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="127" t="s">
-        <v>134</v>
-      </c>
-      <c r="C16" s="127"/>
-      <c r="D16" s="127" t="s">
-        <v>137</v>
-      </c>
-      <c r="E16" s="127" t="s">
-        <v>138</v>
-      </c>
-      <c r="F16" s="127" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="127"/>
-      <c r="H16" s="127"/>
-      <c r="I16" s="127"/>
-      <c r="J16" s="127"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B17" s="127" t="s">
-        <v>134</v>
-      </c>
-      <c r="C17" s="127"/>
-      <c r="D17" s="127" t="s">
-        <v>139</v>
-      </c>
-      <c r="E17" s="127" t="s">
-        <v>140</v>
-      </c>
-      <c r="F17" s="127" t="s">
-        <v>52</v>
-      </c>
-      <c r="G17" s="127"/>
-      <c r="H17" s="127"/>
-      <c r="I17" s="127"/>
-      <c r="J17" s="127"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="127" t="s">
-        <v>134</v>
-      </c>
-      <c r="C18" s="127"/>
-      <c r="D18" s="127" t="s">
-        <v>141</v>
-      </c>
-      <c r="E18" s="127" t="s">
-        <v>142</v>
-      </c>
-      <c r="F18" s="127" t="s">
-        <v>52</v>
-      </c>
-      <c r="G18" s="127"/>
-      <c r="H18" s="127"/>
-      <c r="I18" s="127"/>
-      <c r="J18" s="127"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" s="127" t="s">
-        <v>134</v>
-      </c>
-      <c r="C19" s="127"/>
-      <c r="D19" s="127" t="s">
-        <v>143</v>
-      </c>
-      <c r="E19" s="127" t="s">
-        <v>144</v>
-      </c>
-      <c r="F19" s="127" t="s">
-        <v>52</v>
-      </c>
-      <c r="G19" s="127"/>
-      <c r="H19" s="127"/>
-      <c r="I19" s="127"/>
-      <c r="J19" s="127"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B20" s="127" t="s">
-        <v>134</v>
-      </c>
-      <c r="C20" s="127"/>
-      <c r="D20" s="127" t="s">
-        <v>145</v>
-      </c>
-      <c r="E20" s="127" t="s">
-        <v>146</v>
-      </c>
-      <c r="F20" s="127" t="s">
-        <v>52</v>
-      </c>
-      <c r="G20" s="127"/>
-      <c r="H20" s="127"/>
-      <c r="I20" s="127"/>
-      <c r="J20" s="127"/>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="127" t="s">
-        <v>134</v>
-      </c>
-      <c r="C21" s="127"/>
-      <c r="D21" s="127" t="s">
-        <v>147</v>
-      </c>
-      <c r="E21" s="127" t="s">
-        <v>148</v>
-      </c>
-      <c r="F21" s="127" t="s">
-        <v>52</v>
-      </c>
-      <c r="G21" s="127"/>
-      <c r="H21" s="127"/>
-      <c r="I21" s="127"/>
-      <c r="J21" s="127"/>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B22" s="127" t="s">
-        <v>134</v>
-      </c>
-      <c r="C22" s="127"/>
-      <c r="D22" s="127" t="s">
-        <v>149</v>
-      </c>
-      <c r="E22" s="127" t="s">
-        <v>150</v>
-      </c>
-      <c r="F22" s="127" t="s">
-        <v>52</v>
-      </c>
-      <c r="G22" s="127"/>
-      <c r="H22" s="127"/>
-      <c r="I22" s="127"/>
-      <c r="J22" s="127"/>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B23" s="127" t="s">
-        <v>134</v>
-      </c>
-      <c r="C23" s="127"/>
-      <c r="D23" s="127" t="s">
-        <v>151</v>
-      </c>
-      <c r="E23" s="127" t="s">
-        <v>152</v>
-      </c>
-      <c r="F23" s="127" t="s">
-        <v>52</v>
-      </c>
-      <c r="G23" s="127"/>
-      <c r="H23" s="127"/>
-      <c r="I23" s="127"/>
-      <c r="J23" s="127"/>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B24" s="127" t="s">
-        <v>134</v>
-      </c>
-      <c r="C24" s="127"/>
-      <c r="D24" s="127" t="s">
-        <v>153</v>
-      </c>
-      <c r="E24" s="127" t="s">
-        <v>154</v>
-      </c>
-      <c r="F24" s="127" t="s">
-        <v>52</v>
-      </c>
-      <c r="G24" s="127"/>
-      <c r="H24" s="127"/>
-      <c r="I24" s="127"/>
-      <c r="J24" s="127"/>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B25" s="127" t="s">
-        <v>134</v>
-      </c>
-      <c r="C25" s="127"/>
-      <c r="D25" s="127" t="s">
-        <v>155</v>
-      </c>
-      <c r="E25" s="127" t="s">
-        <v>156</v>
-      </c>
-      <c r="F25" s="127" t="s">
-        <v>52</v>
-      </c>
-      <c r="G25" s="127"/>
-      <c r="H25" s="127"/>
-      <c r="I25" s="127"/>
-      <c r="J25" s="127"/>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B26" s="127" t="s">
-        <v>134</v>
-      </c>
-      <c r="C26" s="127"/>
-      <c r="D26" s="127" t="s">
-        <v>157</v>
-      </c>
-      <c r="E26" s="127" t="s">
-        <v>157</v>
-      </c>
-      <c r="F26" s="127" t="s">
-        <v>52</v>
-      </c>
-      <c r="G26" s="127"/>
-      <c r="H26" s="127"/>
-      <c r="I26" s="127"/>
-      <c r="J26" s="127"/>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B27" s="127" t="s">
-        <v>134</v>
-      </c>
-      <c r="C27" s="127"/>
-      <c r="D27" s="127" t="s">
-        <v>158</v>
-      </c>
-      <c r="E27" s="127" t="s">
-        <v>159</v>
-      </c>
-      <c r="F27" s="127" t="s">
-        <v>52</v>
-      </c>
-      <c r="G27" s="127"/>
-      <c r="H27" s="127"/>
-      <c r="I27" s="127"/>
-      <c r="J27" s="127"/>
-    </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B28" s="127" t="s">
-        <v>134</v>
-      </c>
-      <c r="C28" s="127"/>
-      <c r="D28" s="127" t="s">
-        <v>160</v>
-      </c>
-      <c r="E28" s="127" t="s">
-        <v>161</v>
-      </c>
-      <c r="F28" s="127" t="s">
-        <v>52</v>
-      </c>
-      <c r="G28" s="127"/>
-      <c r="H28" s="127"/>
-      <c r="I28" s="127"/>
-      <c r="J28" s="127"/>
-    </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B29" s="127" t="s">
-        <v>165</v>
-      </c>
-      <c r="C29" s="127"/>
-      <c r="D29" s="127" t="s">
-        <v>162</v>
-      </c>
-      <c r="E29" s="127" t="s">
-        <v>163</v>
-      </c>
-      <c r="F29" s="127" t="s">
-        <v>164</v>
-      </c>
-      <c r="G29" s="127"/>
-      <c r="H29" s="127"/>
-      <c r="I29" s="127"/>
-      <c r="J29" s="127"/>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>134</v>
-      </c>
-      <c r="D30" t="s">
-        <v>56</v>
-      </c>
-      <c r="E30" t="s">
-        <v>173</v>
-      </c>
-      <c r="F30" t="s">
-        <v>52</v>
-      </c>
-      <c r="H30" t="s">
-        <v>176</v>
-      </c>
-      <c r="J30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>165</v>
-      </c>
-      <c r="D31" t="s">
-        <v>174</v>
-      </c>
-      <c r="E31" t="s">
-        <v>175</v>
-      </c>
-      <c r="F31" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B32" s="127" t="s">
-        <v>134</v>
-      </c>
-      <c r="D32" s="127" t="s">
-        <v>177</v>
-      </c>
-      <c r="E32" s="127" t="s">
-        <v>179</v>
-      </c>
-      <c r="F32" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D33" s="127" t="s">
-        <v>178</v>
-      </c>
-      <c r="E33" s="127" t="s">
-        <v>180</v>
-      </c>
-      <c r="F33" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
-        <v>165</v>
-      </c>
-      <c r="D34" s="127" t="s">
-        <v>190</v>
-      </c>
-      <c r="E34" s="127" t="s">
-        <v>191</v>
-      </c>
-      <c r="F34" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -6551,4 +6161,474 @@
   <headerFooter alignWithMargins="0"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50EC31CD-0AC2-4117-ADE4-ED9EFDB1D2DC}">
+  <dimension ref="B3:J27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B3" s="127" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="127"/>
+      <c r="D3" s="127"/>
+      <c r="E3" s="127"/>
+      <c r="F3" s="127"/>
+      <c r="G3" s="127"/>
+      <c r="H3" s="127"/>
+      <c r="I3" s="127"/>
+      <c r="J3" s="127"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="127" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" s="127" t="s">
+        <v>168</v>
+      </c>
+      <c r="E4" s="127" t="s">
+        <v>169</v>
+      </c>
+      <c r="F4" s="127" t="s">
+        <v>170</v>
+      </c>
+      <c r="G4" s="127" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="127" t="s">
+        <v>171</v>
+      </c>
+      <c r="I4" s="127" t="s">
+        <v>131</v>
+      </c>
+      <c r="J4" s="127" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C5" s="127" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="127" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" s="127" t="s">
+        <v>133</v>
+      </c>
+      <c r="F5" s="127" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="127"/>
+      <c r="H5" s="127"/>
+      <c r="I5" s="127"/>
+      <c r="J5" s="127"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C6" s="127" t="s">
+        <v>134</v>
+      </c>
+      <c r="D6" s="127" t="s">
+        <v>135</v>
+      </c>
+      <c r="E6" s="127" t="s">
+        <v>136</v>
+      </c>
+      <c r="F6" s="127" t="s">
+        <v>52</v>
+      </c>
+      <c r="G6" s="127"/>
+      <c r="H6" s="127"/>
+      <c r="I6" s="127"/>
+      <c r="J6" s="127"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C7" s="127" t="s">
+        <v>134</v>
+      </c>
+      <c r="D7" s="127" t="s">
+        <v>137</v>
+      </c>
+      <c r="E7" s="127" t="s">
+        <v>138</v>
+      </c>
+      <c r="F7" s="127" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="127"/>
+      <c r="H7" s="127"/>
+      <c r="I7" s="127"/>
+      <c r="J7" s="127"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C8" s="127" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8" s="127" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" s="127" t="s">
+        <v>140</v>
+      </c>
+      <c r="F8" s="127" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" s="127"/>
+      <c r="H8" s="127"/>
+      <c r="I8" s="127"/>
+      <c r="J8" s="127"/>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C9" s="127" t="s">
+        <v>134</v>
+      </c>
+      <c r="D9" s="127" t="s">
+        <v>141</v>
+      </c>
+      <c r="E9" s="127" t="s">
+        <v>142</v>
+      </c>
+      <c r="F9" s="127" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="127"/>
+      <c r="H9" s="127"/>
+      <c r="I9" s="127"/>
+      <c r="J9" s="127"/>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C10" s="127" t="s">
+        <v>134</v>
+      </c>
+      <c r="D10" s="127" t="s">
+        <v>143</v>
+      </c>
+      <c r="E10" s="127" t="s">
+        <v>144</v>
+      </c>
+      <c r="F10" s="127" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="127"/>
+      <c r="H10" s="127"/>
+      <c r="I10" s="127"/>
+      <c r="J10" s="127"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C11" s="127" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" s="127" t="s">
+        <v>145</v>
+      </c>
+      <c r="E11" s="127" t="s">
+        <v>146</v>
+      </c>
+      <c r="F11" s="127" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="127"/>
+      <c r="H11" s="127"/>
+      <c r="I11" s="127"/>
+      <c r="J11" s="127"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C12" s="127" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" s="127" t="s">
+        <v>147</v>
+      </c>
+      <c r="E12" s="127" t="s">
+        <v>148</v>
+      </c>
+      <c r="F12" s="127" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="127"/>
+      <c r="H12" s="127"/>
+      <c r="I12" s="127"/>
+      <c r="J12" s="127"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C13" s="127" t="s">
+        <v>134</v>
+      </c>
+      <c r="D13" s="127" t="s">
+        <v>149</v>
+      </c>
+      <c r="E13" s="127" t="s">
+        <v>150</v>
+      </c>
+      <c r="F13" s="127" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="127"/>
+      <c r="H13" s="127"/>
+      <c r="I13" s="127"/>
+      <c r="J13" s="127"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C14" s="127" t="s">
+        <v>134</v>
+      </c>
+      <c r="D14" s="127" t="s">
+        <v>151</v>
+      </c>
+      <c r="E14" s="127" t="s">
+        <v>152</v>
+      </c>
+      <c r="F14" s="127" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="127"/>
+      <c r="H14" s="127"/>
+      <c r="I14" s="127"/>
+      <c r="J14" s="127"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C15" s="127" t="s">
+        <v>134</v>
+      </c>
+      <c r="D15" s="127" t="s">
+        <v>153</v>
+      </c>
+      <c r="E15" s="127" t="s">
+        <v>154</v>
+      </c>
+      <c r="F15" s="127" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="127"/>
+      <c r="H15" s="127"/>
+      <c r="I15" s="127"/>
+      <c r="J15" s="127"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C16" s="127" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" s="127" t="s">
+        <v>155</v>
+      </c>
+      <c r="E16" s="127" t="s">
+        <v>156</v>
+      </c>
+      <c r="F16" s="127" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="127"/>
+      <c r="H16" s="127"/>
+      <c r="I16" s="127"/>
+      <c r="J16" s="127"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C17" s="127" t="s">
+        <v>134</v>
+      </c>
+      <c r="D17" s="127" t="s">
+        <v>157</v>
+      </c>
+      <c r="E17" s="127" t="s">
+        <v>157</v>
+      </c>
+      <c r="F17" s="127" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="127"/>
+      <c r="H17" s="127"/>
+      <c r="I17" s="127"/>
+      <c r="J17" s="127"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C18" s="127" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" s="127" t="s">
+        <v>158</v>
+      </c>
+      <c r="E18" s="127" t="s">
+        <v>159</v>
+      </c>
+      <c r="F18" s="127" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="127"/>
+      <c r="H18" s="127"/>
+      <c r="I18" s="127"/>
+      <c r="J18" s="127"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C19" s="127" t="s">
+        <v>134</v>
+      </c>
+      <c r="D19" s="127" t="s">
+        <v>160</v>
+      </c>
+      <c r="E19" s="127" t="s">
+        <v>161</v>
+      </c>
+      <c r="F19" s="127" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" s="127"/>
+      <c r="H19" s="127"/>
+      <c r="I19" s="127"/>
+      <c r="J19" s="127"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C20" s="127" t="s">
+        <v>165</v>
+      </c>
+      <c r="D20" s="127" t="s">
+        <v>162</v>
+      </c>
+      <c r="E20" s="127" t="s">
+        <v>163</v>
+      </c>
+      <c r="F20" s="127" t="s">
+        <v>164</v>
+      </c>
+      <c r="G20" s="127"/>
+      <c r="H20" s="127"/>
+      <c r="I20" s="127"/>
+      <c r="J20" s="127"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" t="s">
+        <v>173</v>
+      </c>
+      <c r="F21" t="s">
+        <v>52</v>
+      </c>
+      <c r="H21" t="s">
+        <v>176</v>
+      </c>
+      <c r="J21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>165</v>
+      </c>
+      <c r="D22" t="s">
+        <v>174</v>
+      </c>
+      <c r="E22" t="s">
+        <v>175</v>
+      </c>
+      <c r="F22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C23" s="127" t="s">
+        <v>134</v>
+      </c>
+      <c r="D23" s="127" t="s">
+        <v>177</v>
+      </c>
+      <c r="E23" s="127" t="s">
+        <v>179</v>
+      </c>
+      <c r="F23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="D24" s="127" t="s">
+        <v>178</v>
+      </c>
+      <c r="E24" s="127" t="s">
+        <v>180</v>
+      </c>
+      <c r="F24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>165</v>
+      </c>
+      <c r="D25" s="127" t="s">
+        <v>190</v>
+      </c>
+      <c r="E25" s="127" t="s">
+        <v>191</v>
+      </c>
+      <c r="F25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>201</v>
+      </c>
+      <c r="C26" t="s">
+        <v>134</v>
+      </c>
+      <c r="D26" s="127" t="s">
+        <v>203</v>
+      </c>
+      <c r="E26" s="127" t="s">
+        <v>205</v>
+      </c>
+      <c r="F26" t="s">
+        <v>52</v>
+      </c>
+      <c r="H26" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>202</v>
+      </c>
+      <c r="C27" t="s">
+        <v>165</v>
+      </c>
+      <c r="D27" s="127" t="s">
+        <v>203</v>
+      </c>
+      <c r="E27" s="127" t="s">
+        <v>206</v>
+      </c>
+      <c r="F27" t="s">
+        <v>164</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
cases for determining a single pcg when there are multiple commodities in trade processes
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA\VEDA_Models\Demo_Adv_Veda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\Demo_Adv_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA02264D-595B-45BB-A664-007BBAFCAC3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC0F735-2F65-4B40-B469-2D9456390537}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="853" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" tabRatio="853" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region-Time Slices" sheetId="16" r:id="rId1"/>
@@ -29,17 +29,7 @@
   <definedNames>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -261,7 +251,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="213">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -882,6 +872,24 @@
   </si>
   <si>
     <t>commodity x in non-elc regions</t>
+  </si>
+  <si>
+    <t>ENVt</t>
+  </si>
+  <si>
+    <t>NRGt</t>
+  </si>
+  <si>
+    <t>MATt</t>
+  </si>
+  <si>
+    <t>FINt</t>
+  </si>
+  <si>
+    <t>DEMt</t>
+  </si>
+  <si>
+    <t>mUSD</t>
   </si>
 </sst>
 </file>
@@ -6165,10 +6173,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50EC31CD-0AC2-4117-ADE4-ED9EFDB1D2DC}">
-  <dimension ref="B3:J27"/>
+  <dimension ref="B3:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6626,6 +6634,86 @@
         <v>164</v>
       </c>
     </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C28" t="str">
+        <f>LEFT(D28,3)</f>
+        <v>ENV</v>
+      </c>
+      <c r="D28" s="127" t="s">
+        <v>207</v>
+      </c>
+      <c r="E28" t="str">
+        <f>C28&amp;" commodity to test trade pcg"</f>
+        <v>ENV commodity to test trade pcg</v>
+      </c>
+      <c r="F28" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C29" t="str">
+        <f t="shared" ref="C29:C32" si="0">LEFT(D29,3)</f>
+        <v>NRG</v>
+      </c>
+      <c r="D29" s="127" t="s">
+        <v>208</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" ref="E29:E32" si="1">C29&amp;" commodity to test trade pcg"</f>
+        <v>NRG commodity to test trade pcg</v>
+      </c>
+      <c r="F29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>MAT</v>
+      </c>
+      <c r="D30" s="127" t="s">
+        <v>209</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="1"/>
+        <v>MAT commodity to test trade pcg</v>
+      </c>
+      <c r="F30" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>FIN</v>
+      </c>
+      <c r="D31" s="127" t="s">
+        <v>210</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="1"/>
+        <v>FIN commodity to test trade pcg</v>
+      </c>
+      <c r="F31" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>DEM</v>
+      </c>
+      <c r="D32" s="127" t="s">
+        <v>211</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="1"/>
+        <v>DEM commodity to test trade pcg</v>
+      </c>
+      <c r="F32" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
some cleanup of syssettings; including jobs accounting example
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda\Veda_models\Demo_Adv_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CCB27A8-0B08-4A21-BE0E-537C3A849A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CAD1E1E-2B49-4500-A1C8-C14B6E6F7BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="2985" windowWidth="21600" windowHeight="12735" tabRatio="853" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="853" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region-Time Slices" sheetId="16" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Sheet1" sheetId="23" r:id="rId5"/>
     <sheet name="Constants" sheetId="20" r:id="rId6"/>
     <sheet name="TimeSlices" sheetId="22" r:id="rId7"/>
-    <sheet name="Sheet2" sheetId="26" r:id="rId8"/>
+    <sheet name="reporting options" sheetId="26" r:id="rId8"/>
     <sheet name="Defaults" sheetId="21" r:id="rId9"/>
     <sheet name="Commodity Group" sheetId="15" r:id="rId10"/>
     <sheet name="Commodities" sheetId="24" r:id="rId11"/>
@@ -265,7 +265,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="294">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -1134,36 +1134,6 @@
     <t>OBJ~1</t>
   </si>
   <si>
-    <t>~RFInput</t>
-  </si>
-  <si>
-    <t>Sno</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>RFSwitch</t>
-  </si>
-  <si>
-    <t>$SET BENCOST YES</t>
-  </si>
-  <si>
-    <t>benefit-cost reporting for new technologies</t>
-  </si>
-  <si>
-    <t>$SET ANNCOST LEV</t>
-  </si>
-  <si>
-    <t>report annual costs based upon levelized values over process lifetimes or periods</t>
-  </si>
-  <si>
-    <t>$SET WAVER YES</t>
-  </si>
-  <si>
-    <t>weighted average interpolation (COM_PROJ and PRC_RESID)</t>
-  </si>
-  <si>
     <t>FLO~1</t>
   </si>
   <si>
@@ -1174,6 +1144,9 @@
   </si>
   <si>
     <t>~-1</t>
+  </si>
+  <si>
+    <t>Def5</t>
   </si>
 </sst>
 </file>
@@ -2805,7 +2778,7 @@
     <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3108,6 +3081,7 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="431" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="431" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="431" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="435">
     <cellStyle name="20% - Accent1 2" xfId="9" xr:uid="{868B5B88-E909-4783-AD13-DE2EB64A3CB4}"/>
@@ -5883,7 +5857,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -7134,9 +7108,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:E39"/>
+  <dimension ref="A3:F39"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -7232,7 +7208,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:6">
       <c r="B17" s="14"/>
       <c r="C17" s="14">
         <v>5</v>
@@ -7241,54 +7217,54 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:6">
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
       <c r="D19" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:6">
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
       <c r="D20" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:6">
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
       <c r="D21" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:6">
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
       <c r="D22" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:6">
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
       <c r="D23" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:6">
       <c r="A26" s="129" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>217</v>
       </c>
@@ -7304,8 +7280,11 @@
       <c r="E27" s="125" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27" s="138" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>246</v>
       </c>
@@ -7322,7 +7301,7 @@
         <v>2054</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>247</v>
       </c>
@@ -7338,8 +7317,11 @@
       <c r="E29" s="14">
         <v>2005</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29" s="14">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>247</v>
       </c>
@@ -7355,8 +7337,11 @@
       <c r="E30" s="14">
         <v>2006</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30" s="14">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>247</v>
       </c>
@@ -7370,8 +7355,11 @@
       <c r="E31" s="14">
         <v>2007</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31" s="14">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>247</v>
       </c>
@@ -7385,8 +7373,11 @@
       <c r="E32" s="14">
         <v>2010</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32" s="14">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>247</v>
       </c>
@@ -7400,8 +7391,11 @@
       <c r="E33" s="14">
         <v>2015</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33" s="14">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>247</v>
       </c>
@@ -7413,8 +7407,11 @@
       <c r="E34" s="14">
         <v>2020</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34" s="14">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>247</v>
       </c>
@@ -7426,8 +7423,11 @@
       <c r="E35" s="14">
         <v>2030</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35" s="14">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>247</v>
       </c>
@@ -7439,8 +7439,11 @@
       <c r="E36" s="14">
         <v>2050</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36" s="14">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>247</v>
       </c>
@@ -7450,8 +7453,11 @@
       <c r="E37" s="14">
         <v>2060</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37" s="14">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>247</v>
       </c>
@@ -7461,8 +7467,11 @@
       <c r="E38" s="14">
         <v>2075</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38" s="14">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>247</v>
       </c>
@@ -7471,6 +7480,9 @@
       <c r="D39" s="14"/>
       <c r="E39" s="14">
         <v>2100</v>
+      </c>
+      <c r="F39" s="14">
+        <v>2050</v>
       </c>
     </row>
   </sheetData>
@@ -7486,7 +7498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -7572,7 +7584,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="19.5" customHeight="1"/>
@@ -8869,7 +8881,7 @@
   <dimension ref="B4:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -8912,7 +8924,7 @@
         <v>282</v>
       </c>
       <c r="D7" s="134" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="E7" s="134">
         <v>1</v>
@@ -8983,88 +8995,22 @@
         <v>282</v>
       </c>
       <c r="D13" s="134" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="E13" s="134">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:10">
-      <c r="B17" s="136" t="s">
-        <v>289</v>
-      </c>
-      <c r="C17" s="134"/>
-      <c r="D17" s="134"/>
-      <c r="E17" s="134"/>
-    </row>
-    <row r="18" spans="2:10">
-      <c r="B18" s="135" t="s">
-        <v>290</v>
-      </c>
-      <c r="C18" s="135" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" s="135" t="s">
-        <v>291</v>
-      </c>
-      <c r="E18" s="134"/>
-      <c r="F18" s="133"/>
-      <c r="G18" s="133"/>
-      <c r="H18" s="133"/>
-      <c r="I18" s="133"/>
+    <row r="18" spans="10:10">
       <c r="J18" s="133"/>
     </row>
-    <row r="19" spans="2:10">
-      <c r="B19" s="134">
-        <v>1</v>
-      </c>
-      <c r="C19" s="134" t="s">
-        <v>292</v>
-      </c>
-      <c r="D19" s="134" t="s">
-        <v>293</v>
-      </c>
-      <c r="E19" s="134"/>
-      <c r="F19" s="134"/>
-      <c r="G19" s="134" t="s">
-        <v>294</v>
-      </c>
-      <c r="H19" s="134"/>
-      <c r="I19" s="134"/>
+    <row r="19" spans="10:10">
       <c r="J19" s="134"/>
     </row>
-    <row r="20" spans="2:10">
-      <c r="B20" s="134"/>
-      <c r="C20" s="134" t="s">
-        <v>292</v>
-      </c>
-      <c r="D20" s="134" t="s">
-        <v>295</v>
-      </c>
-      <c r="E20" s="134"/>
-      <c r="F20" s="134"/>
-      <c r="G20" s="134" t="s">
-        <v>296</v>
-      </c>
-      <c r="H20" s="134"/>
-      <c r="I20" s="134"/>
+    <row r="20" spans="10:10">
       <c r="J20" s="134"/>
     </row>
-    <row r="21" spans="2:10">
-      <c r="B21" s="134"/>
-      <c r="C21" s="134" t="s">
-        <v>292</v>
-      </c>
-      <c r="D21" s="134" t="s">
-        <v>297</v>
-      </c>
-      <c r="E21" s="134"/>
-      <c r="F21" s="134"/>
-      <c r="G21" s="134" t="s">
-        <v>298</v>
-      </c>
-      <c r="H21" s="134"/>
-      <c r="I21" s="134"/>
+    <row r="21" spans="10:10">
       <c r="J21" s="134"/>
     </row>
   </sheetData>
@@ -9418,7 +9364,7 @@
         <v>80</v>
       </c>
       <c r="C33" s="131" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="D33" s="130">
         <v>1000</v>

</xml_diff>

<commit_message>
added new def7 to make bigger models
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda\Veda_models\Demo_Adv_Veda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VEDA_Release\Model_Demo_Adv_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9751AD3C-B5BE-47E4-B719-8EE4E525D087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211D514F-B4CC-495D-B369-C780552050D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="853" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="853" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region-Time Slices" sheetId="16" r:id="rId1"/>
@@ -32,14 +32,12 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Defaults!$B$14:$D$32</definedName>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -265,7 +263,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="304">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -1174,6 +1172,9 @@
   </si>
   <si>
     <t>ACT~2</t>
+  </si>
+  <si>
+    <t>Def7</t>
   </si>
 </sst>
 </file>
@@ -7193,10 +7194,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:G39"/>
+  <dimension ref="A3:H79"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="Q65" sqref="Q65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -7293,7 +7294,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8">
       <c r="B17" s="14"/>
       <c r="C17" s="14">
         <v>5</v>
@@ -7302,54 +7303,54 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:8">
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:8">
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
       <c r="D19" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:8">
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
       <c r="D20" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:8">
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
       <c r="D21" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:8">
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
       <c r="D22" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:8">
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
       <c r="D23" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:8">
       <c r="A26" s="129" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>217</v>
       </c>
@@ -7371,8 +7372,11 @@
       <c r="G27" s="138" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="H27" s="138" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>246</v>
       </c>
@@ -7389,7 +7393,7 @@
         <v>2054</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>247</v>
       </c>
@@ -7411,8 +7415,11 @@
       <c r="G29" s="14">
         <v>2005</v>
       </c>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="H29" s="14">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>247</v>
       </c>
@@ -7434,8 +7441,11 @@
       <c r="G30" s="14">
         <v>2010</v>
       </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="H30" s="14">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>247</v>
       </c>
@@ -7455,8 +7465,11 @@
       <c r="G31" s="14">
         <v>2020</v>
       </c>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="H31" s="14">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>247</v>
       </c>
@@ -7476,8 +7489,11 @@
       <c r="G32" s="14">
         <v>2025</v>
       </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="H32" s="14">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>247</v>
       </c>
@@ -7497,8 +7513,11 @@
       <c r="G33" s="14">
         <v>2030</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="H33" s="14">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>247</v>
       </c>
@@ -7516,8 +7535,11 @@
       <c r="G34" s="14">
         <v>2035</v>
       </c>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="H34" s="14">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>247</v>
       </c>
@@ -7535,8 +7557,11 @@
       <c r="G35" s="14">
         <v>2040</v>
       </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="H35" s="14">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>247</v>
       </c>
@@ -7554,8 +7579,11 @@
       <c r="G36" s="14">
         <v>2045</v>
       </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="H36" s="14">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>247</v>
       </c>
@@ -7571,8 +7599,11 @@
       <c r="G37" s="14">
         <v>2050</v>
       </c>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="H37" s="14">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38" t="s">
         <v>247</v>
       </c>
@@ -7586,8 +7617,11 @@
         <v>2040</v>
       </c>
       <c r="G38" s="14"/>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="H38" s="14">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" t="s">
         <v>247</v>
       </c>
@@ -7601,6 +7635,207 @@
         <v>2050</v>
       </c>
       <c r="G39" s="14"/>
+      <c r="H39" s="14">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="H40" s="14">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="H41" s="14">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="H42" s="14">
+        <v>2014</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="H43" s="14">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="H44" s="14">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="H45" s="14">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="H46" s="14">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="H47" s="14">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="H48" s="14">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="49" spans="8:8">
+      <c r="H49" s="14">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="50" spans="8:8">
+      <c r="H50" s="14">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="51" spans="8:8">
+      <c r="H51" s="14">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="52" spans="8:8">
+      <c r="H52" s="14">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="53" spans="8:8">
+      <c r="H53" s="14">
+        <v>2025</v>
+      </c>
+    </row>
+    <row r="54" spans="8:8">
+      <c r="H54" s="14">
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="55" spans="8:8">
+      <c r="H55" s="14">
+        <v>2027</v>
+      </c>
+    </row>
+    <row r="56" spans="8:8">
+      <c r="H56" s="14">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="57" spans="8:8">
+      <c r="H57" s="14">
+        <v>2029</v>
+      </c>
+    </row>
+    <row r="58" spans="8:8">
+      <c r="H58" s="14">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="59" spans="8:8">
+      <c r="H59" s="14">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="60" spans="8:8">
+      <c r="H60" s="14">
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="61" spans="8:8">
+      <c r="H61" s="14">
+        <v>2033</v>
+      </c>
+    </row>
+    <row r="62" spans="8:8">
+      <c r="H62" s="14">
+        <v>2034</v>
+      </c>
+    </row>
+    <row r="63" spans="8:8">
+      <c r="H63" s="14">
+        <v>2035</v>
+      </c>
+    </row>
+    <row r="64" spans="8:8">
+      <c r="H64" s="14">
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="65" spans="8:8">
+      <c r="H65" s="14">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="66" spans="8:8">
+      <c r="H66" s="14">
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="67" spans="8:8">
+      <c r="H67" s="14">
+        <v>2039</v>
+      </c>
+    </row>
+    <row r="68" spans="8:8">
+      <c r="H68" s="14">
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="69" spans="8:8">
+      <c r="H69" s="14">
+        <v>2041</v>
+      </c>
+    </row>
+    <row r="70" spans="8:8">
+      <c r="H70" s="14">
+        <v>2042</v>
+      </c>
+    </row>
+    <row r="71" spans="8:8">
+      <c r="H71" s="14">
+        <v>2043</v>
+      </c>
+    </row>
+    <row r="72" spans="8:8">
+      <c r="H72" s="14">
+        <v>2044</v>
+      </c>
+    </row>
+    <row r="73" spans="8:8">
+      <c r="H73" s="14">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="74" spans="8:8">
+      <c r="H74" s="14">
+        <v>2046</v>
+      </c>
+    </row>
+    <row r="75" spans="8:8">
+      <c r="H75" s="14">
+        <v>2047</v>
+      </c>
+    </row>
+    <row r="76" spans="8:8">
+      <c r="H76" s="14">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="77" spans="8:8">
+      <c r="H77" s="14">
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="78" spans="8:8">
+      <c r="H78" s="14">
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="79" spans="8:8">
+      <c r="H79" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -8997,7 +9232,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8848E86-A146-4530-A694-2F38523B621A}">
   <dimension ref="B4:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
setting up Timeslices def in scenario files
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda\Veda_models\Demo_Adv_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5122A9A7-87C9-4AC7-AB0B-26F2CF4FBAC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD6619D-1925-409E-97B7-D871546CB7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30780" yWindow="2850" windowWidth="21600" windowHeight="14565" tabRatio="853" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4590" yWindow="2160" windowWidth="21600" windowHeight="15165" tabRatio="853" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region-Time Slices" sheetId="16" r:id="rId1"/>
@@ -265,7 +265,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="293">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -1141,6 +1141,9 @@
   </si>
   <si>
     <t>ACT~2</t>
+  </si>
+  <si>
+    <t>ELC~3</t>
   </si>
 </sst>
 </file>
@@ -6124,7 +6127,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="B1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -8948,8 +8951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8848E86-A146-4530-A694-2F38523B621A}">
   <dimension ref="B4:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -9081,6 +9084,17 @@
       </c>
       <c r="E14" s="139">
         <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="C15" t="s">
+        <v>278</v>
+      </c>
+      <c r="D15" t="s">
+        <v>292</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="10:10">

</xml_diff>

<commit_message>
creating an example to model limited time PTC
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda\Veda_models\Demo_Adv_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD6619D-1925-409E-97B7-D871546CB7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30AA9FE6-AB83-4492-B244-C7DCA19C8173}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="2160" windowWidth="21600" windowHeight="15165" tabRatio="853" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="12735" tabRatio="853" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region-Time Slices" sheetId="16" r:id="rId1"/>
@@ -265,7 +265,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="295">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -1144,6 +1144,12 @@
   </si>
   <si>
     <t>ELC~3</t>
+  </si>
+  <si>
+    <t>PTC</t>
+  </si>
+  <si>
+    <t>to model production tax credit</t>
   </si>
 </sst>
 </file>
@@ -2775,17 +2781,16 @@
     <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="140">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2795,29 +2800,25 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFill="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="6" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="6" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="5" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2845,10 +2846,8 @@
     <xf numFmtId="165" fontId="2" fillId="4" borderId="10" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2860,11 +2859,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="4" borderId="11" xfId="6" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2873,7 +2871,7 @@
     <xf numFmtId="2" fontId="6" fillId="4" borderId="11" xfId="6" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="6" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="6" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2891,19 +2889,19 @@
     <xf numFmtId="2" fontId="6" fillId="4" borderId="8" xfId="6" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="6" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="6" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2921,10 +2919,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="6" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2936,7 +2931,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2966,9 +2961,8 @@
     <xf numFmtId="165" fontId="13" fillId="4" borderId="10" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2980,11 +2974,10 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="10" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="14" fillId="4" borderId="11" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3014,16 +3007,16 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="8" xfId="6" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="14" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="7" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3047,10 +3040,7 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="11" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="14" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3071,15 +3061,11 @@
     <xf numFmtId="0" fontId="20" fillId="8" borderId="15" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="431"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="431" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="64" fillId="0" borderId="0" xfId="431" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="431" applyFont="1"/>
     <xf numFmtId="0" fontId="63" fillId="0" borderId="0" xfId="421"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="431" applyFill="1"/>
   </cellXfs>
   <cellStyles count="435">
     <cellStyle name="20% - Accent1 2" xfId="9" xr:uid="{868B5B88-E909-4783-AD13-DE2EB64A3CB4}"/>
@@ -5853,7 +5839,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N38"/>
+  <dimension ref="B1:N17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -5866,18 +5852,17 @@
     <col min="8" max="8" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="2:14">
       <c r="N1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="2:14">
       <c r="N2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="6"/>
+    <row r="3" spans="2:14">
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
@@ -5885,8 +5870,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="6"/>
+    <row r="4" spans="2:14">
       <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
@@ -5903,215 +5887,127 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="6"/>
-      <c r="B5" s="15" t="s">
+    <row r="5" spans="2:14">
+      <c r="B5" s="14" t="s">
         <v>48</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" t="s">
         <v>68</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6" t="s">
+      <c r="J5" t="s">
         <v>71</v>
       </c>
       <c r="N5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="6"/>
-      <c r="B6" s="15" t="s">
+    <row r="6" spans="2:14">
+      <c r="B6" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" t="s">
         <v>88</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6" t="s">
+      <c r="J6" t="s">
         <v>72</v>
       </c>
       <c r="N6" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
-      <c r="A7" s="6"/>
-      <c r="B7" s="15" t="s">
+    <row r="7" spans="2:14">
+      <c r="B7" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" t="s">
         <v>120</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" t="s">
         <v>70</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" t="s">
         <v>87</v>
       </c>
       <c r="N7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6" t="s">
+    <row r="8" spans="2:14">
+      <c r="C8" t="s">
         <v>121</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" t="s">
         <v>95</v>
       </c>
       <c r="N8" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6" t="s">
+    <row r="9" spans="2:14">
+      <c r="C9" t="s">
         <v>122</v>
       </c>
       <c r="N9" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6" t="s">
+    <row r="10" spans="2:14">
+      <c r="C10" t="s">
         <v>123</v>
       </c>
       <c r="N10" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6" t="s">
+    <row r="11" spans="2:14">
+      <c r="B11" t="s">
         <v>129</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" t="s">
         <v>124</v>
       </c>
       <c r="N11" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6" t="s">
+    <row r="12" spans="2:14">
+      <c r="C12" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6" t="s">
+    <row r="13" spans="2:14">
+      <c r="C13" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6" t="s">
+    <row r="14" spans="2:14">
+      <c r="C14" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6" t="s">
+    <row r="15" spans="2:14">
+      <c r="B15" t="s">
         <v>186</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6" t="s">
+    <row r="16" spans="2:14">
+      <c r="C16" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6" t="s">
+    <row r="17" spans="3:3">
+      <c r="C17" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="6"/>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="6"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="6"/>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="6"/>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="6"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="6"/>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="6"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="6"/>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="6"/>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="6"/>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="6"/>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="6"/>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="6"/>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="6"/>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="6"/>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="6"/>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="6"/>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="6"/>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="6"/>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -6125,7 +6021,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="B1:I17"/>
+  <dimension ref="B2:I17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
@@ -6145,34 +6041,25 @@
     <col min="10" max="11" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9">
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-    </row>
     <row r="2" spans="2:9" ht="15">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
     </row>
     <row r="4" spans="2:9" ht="21" customHeight="1">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" spans="2:9" ht="18" customHeight="1">
       <c r="B5" s="1" t="s">
@@ -6206,18 +6093,18 @@
       </c>
     </row>
     <row r="7" spans="2:9" ht="26.25" thickBot="1">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
     </row>
     <row r="8" spans="2:9">
       <c r="B8" t="s">
@@ -6254,17 +6141,17 @@
       </c>
     </row>
     <row r="14" spans="2:9">
-      <c r="B14" s="132"/>
+      <c r="B14" s="119"/>
     </row>
     <row r="16" spans="2:9">
-      <c r="B16" s="138"/>
-      <c r="C16" s="138"/>
-      <c r="D16" s="138"/>
+      <c r="B16" s="123"/>
+      <c r="C16" s="123"/>
+      <c r="D16" s="123"/>
     </row>
     <row r="17" spans="2:4">
-      <c r="B17" s="138"/>
-      <c r="C17" s="138"/>
-      <c r="D17" s="138"/>
+      <c r="B17" s="123"/>
+      <c r="C17" s="123"/>
+      <c r="D17" s="123"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -6277,10 +6164,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50EC31CD-0AC2-4117-ADE4-ED9EFDB1D2DC}">
-  <dimension ref="B3:J33"/>
+  <dimension ref="B3:J34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6299,334 +6186,334 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:10">
-      <c r="B3" s="124" t="s">
+      <c r="B3" s="112" t="s">
         <v>165</v>
       </c>
-      <c r="C3" s="124"/>
-      <c r="D3" s="124"/>
-      <c r="E3" s="124"/>
-      <c r="F3" s="124"/>
-      <c r="G3" s="124"/>
-      <c r="H3" s="124"/>
-      <c r="I3" s="124"/>
-      <c r="J3" s="124"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="112"/>
+      <c r="I3" s="112"/>
+      <c r="J3" s="112"/>
     </row>
     <row r="4" spans="2:10">
       <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="124" t="s">
+      <c r="C4" s="112" t="s">
         <v>166</v>
       </c>
-      <c r="D4" s="124" t="s">
+      <c r="D4" s="112" t="s">
         <v>167</v>
       </c>
-      <c r="E4" s="124" t="s">
+      <c r="E4" s="112" t="s">
         <v>168</v>
       </c>
-      <c r="F4" s="124" t="s">
+      <c r="F4" s="112" t="s">
         <v>169</v>
       </c>
-      <c r="G4" s="124" t="s">
+      <c r="G4" s="112" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="124" t="s">
+      <c r="H4" s="112" t="s">
         <v>170</v>
       </c>
-      <c r="I4" s="124" t="s">
+      <c r="I4" s="112" t="s">
         <v>130</v>
       </c>
-      <c r="J4" s="124" t="s">
+      <c r="J4" s="112" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="5" spans="2:10">
-      <c r="C5" s="124" t="s">
+      <c r="C5" s="112" t="s">
         <v>133</v>
       </c>
-      <c r="D5" s="124" t="s">
+      <c r="D5" s="112" t="s">
         <v>131</v>
       </c>
-      <c r="E5" s="124" t="s">
+      <c r="E5" s="112" t="s">
         <v>132</v>
       </c>
-      <c r="F5" s="124" t="s">
+      <c r="F5" s="112" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="124"/>
-      <c r="H5" s="124"/>
-      <c r="I5" s="124"/>
-      <c r="J5" s="124"/>
+      <c r="G5" s="112"/>
+      <c r="H5" s="112"/>
+      <c r="I5" s="112"/>
+      <c r="J5" s="112"/>
     </row>
     <row r="6" spans="2:10">
-      <c r="C6" s="124" t="s">
+      <c r="C6" s="112" t="s">
         <v>133</v>
       </c>
-      <c r="D6" s="124" t="s">
+      <c r="D6" s="112" t="s">
         <v>134</v>
       </c>
-      <c r="E6" s="124" t="s">
+      <c r="E6" s="112" t="s">
         <v>135</v>
       </c>
-      <c r="F6" s="124" t="s">
+      <c r="F6" s="112" t="s">
         <v>51</v>
       </c>
-      <c r="G6" s="124"/>
-      <c r="H6" s="124"/>
-      <c r="I6" s="124"/>
-      <c r="J6" s="124"/>
+      <c r="G6" s="112"/>
+      <c r="H6" s="112"/>
+      <c r="I6" s="112"/>
+      <c r="J6" s="112"/>
     </row>
     <row r="7" spans="2:10">
-      <c r="C7" s="124" t="s">
+      <c r="C7" s="112" t="s">
         <v>133</v>
       </c>
-      <c r="D7" s="124" t="s">
+      <c r="D7" s="112" t="s">
         <v>136</v>
       </c>
-      <c r="E7" s="124" t="s">
+      <c r="E7" s="112" t="s">
         <v>137</v>
       </c>
-      <c r="F7" s="124" t="s">
+      <c r="F7" s="112" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="124"/>
-      <c r="H7" s="124"/>
-      <c r="I7" s="124"/>
-      <c r="J7" s="124"/>
+      <c r="G7" s="112"/>
+      <c r="H7" s="112"/>
+      <c r="I7" s="112"/>
+      <c r="J7" s="112"/>
     </row>
     <row r="8" spans="2:10">
-      <c r="C8" s="124" t="s">
+      <c r="C8" s="112" t="s">
         <v>133</v>
       </c>
-      <c r="D8" s="124" t="s">
+      <c r="D8" s="112" t="s">
         <v>138</v>
       </c>
-      <c r="E8" s="124" t="s">
+      <c r="E8" s="112" t="s">
         <v>139</v>
       </c>
-      <c r="F8" s="124" t="s">
+      <c r="F8" s="112" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="124"/>
-      <c r="H8" s="124"/>
-      <c r="I8" s="124"/>
-      <c r="J8" s="124"/>
+      <c r="G8" s="112"/>
+      <c r="H8" s="112"/>
+      <c r="I8" s="112"/>
+      <c r="J8" s="112"/>
     </row>
     <row r="9" spans="2:10">
-      <c r="C9" s="124" t="s">
+      <c r="C9" s="112" t="s">
         <v>133</v>
       </c>
-      <c r="D9" s="124" t="s">
+      <c r="D9" s="112" t="s">
         <v>140</v>
       </c>
-      <c r="E9" s="124" t="s">
+      <c r="E9" s="112" t="s">
         <v>141</v>
       </c>
-      <c r="F9" s="124" t="s">
+      <c r="F9" s="112" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="124"/>
-      <c r="H9" s="124"/>
-      <c r="I9" s="124"/>
-      <c r="J9" s="124"/>
+      <c r="G9" s="112"/>
+      <c r="H9" s="112"/>
+      <c r="I9" s="112"/>
+      <c r="J9" s="112"/>
     </row>
     <row r="10" spans="2:10">
-      <c r="C10" s="124" t="s">
+      <c r="C10" s="112" t="s">
         <v>133</v>
       </c>
-      <c r="D10" s="124" t="s">
+      <c r="D10" s="112" t="s">
         <v>142</v>
       </c>
-      <c r="E10" s="124" t="s">
+      <c r="E10" s="112" t="s">
         <v>143</v>
       </c>
-      <c r="F10" s="124" t="s">
+      <c r="F10" s="112" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="124"/>
-      <c r="H10" s="124"/>
-      <c r="I10" s="124"/>
-      <c r="J10" s="124"/>
+      <c r="G10" s="112"/>
+      <c r="H10" s="112"/>
+      <c r="I10" s="112"/>
+      <c r="J10" s="112"/>
     </row>
     <row r="11" spans="2:10">
-      <c r="C11" s="124" t="s">
+      <c r="C11" s="112" t="s">
         <v>133</v>
       </c>
-      <c r="D11" s="124" t="s">
+      <c r="D11" s="112" t="s">
         <v>144</v>
       </c>
-      <c r="E11" s="124" t="s">
+      <c r="E11" s="112" t="s">
         <v>145</v>
       </c>
-      <c r="F11" s="124" t="s">
+      <c r="F11" s="112" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="124"/>
-      <c r="H11" s="124"/>
-      <c r="I11" s="124"/>
-      <c r="J11" s="124"/>
+      <c r="G11" s="112"/>
+      <c r="H11" s="112"/>
+      <c r="I11" s="112"/>
+      <c r="J11" s="112"/>
     </row>
     <row r="12" spans="2:10">
-      <c r="C12" s="124" t="s">
+      <c r="C12" s="112" t="s">
         <v>133</v>
       </c>
-      <c r="D12" s="124" t="s">
+      <c r="D12" s="112" t="s">
         <v>146</v>
       </c>
-      <c r="E12" s="124" t="s">
+      <c r="E12" s="112" t="s">
         <v>147</v>
       </c>
-      <c r="F12" s="124" t="s">
+      <c r="F12" s="112" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="124"/>
-      <c r="H12" s="124"/>
-      <c r="I12" s="124"/>
-      <c r="J12" s="124"/>
+      <c r="G12" s="112"/>
+      <c r="H12" s="112"/>
+      <c r="I12" s="112"/>
+      <c r="J12" s="112"/>
     </row>
     <row r="13" spans="2:10">
-      <c r="C13" s="124" t="s">
+      <c r="C13" s="112" t="s">
         <v>133</v>
       </c>
-      <c r="D13" s="124" t="s">
+      <c r="D13" s="112" t="s">
         <v>148</v>
       </c>
-      <c r="E13" s="124" t="s">
+      <c r="E13" s="112" t="s">
         <v>149</v>
       </c>
-      <c r="F13" s="124" t="s">
+      <c r="F13" s="112" t="s">
         <v>51</v>
       </c>
-      <c r="G13" s="124"/>
-      <c r="H13" s="124"/>
-      <c r="I13" s="124"/>
-      <c r="J13" s="124"/>
+      <c r="G13" s="112"/>
+      <c r="H13" s="112"/>
+      <c r="I13" s="112"/>
+      <c r="J13" s="112"/>
     </row>
     <row r="14" spans="2:10">
-      <c r="C14" s="124" t="s">
+      <c r="C14" s="112" t="s">
         <v>133</v>
       </c>
-      <c r="D14" s="124" t="s">
+      <c r="D14" s="112" t="s">
         <v>150</v>
       </c>
-      <c r="E14" s="124" t="s">
+      <c r="E14" s="112" t="s">
         <v>151</v>
       </c>
-      <c r="F14" s="124" t="s">
+      <c r="F14" s="112" t="s">
         <v>51</v>
       </c>
-      <c r="G14" s="124"/>
-      <c r="H14" s="124"/>
-      <c r="I14" s="124"/>
-      <c r="J14" s="124"/>
+      <c r="G14" s="112"/>
+      <c r="H14" s="112"/>
+      <c r="I14" s="112"/>
+      <c r="J14" s="112"/>
     </row>
     <row r="15" spans="2:10">
-      <c r="C15" s="124" t="s">
+      <c r="C15" s="112" t="s">
         <v>133</v>
       </c>
-      <c r="D15" s="124" t="s">
+      <c r="D15" s="112" t="s">
         <v>152</v>
       </c>
-      <c r="E15" s="124" t="s">
+      <c r="E15" s="112" t="s">
         <v>153</v>
       </c>
-      <c r="F15" s="124" t="s">
+      <c r="F15" s="112" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="124"/>
-      <c r="H15" s="124"/>
-      <c r="I15" s="124"/>
-      <c r="J15" s="124"/>
+      <c r="G15" s="112"/>
+      <c r="H15" s="112"/>
+      <c r="I15" s="112"/>
+      <c r="J15" s="112"/>
     </row>
     <row r="16" spans="2:10">
-      <c r="C16" s="124" t="s">
+      <c r="C16" s="112" t="s">
         <v>133</v>
       </c>
-      <c r="D16" s="124" t="s">
+      <c r="D16" s="112" t="s">
         <v>154</v>
       </c>
-      <c r="E16" s="124" t="s">
+      <c r="E16" s="112" t="s">
         <v>155</v>
       </c>
-      <c r="F16" s="124" t="s">
+      <c r="F16" s="112" t="s">
         <v>51</v>
       </c>
-      <c r="G16" s="124"/>
-      <c r="H16" s="124"/>
-      <c r="I16" s="124"/>
-      <c r="J16" s="124"/>
+      <c r="G16" s="112"/>
+      <c r="H16" s="112"/>
+      <c r="I16" s="112"/>
+      <c r="J16" s="112"/>
     </row>
     <row r="17" spans="2:10">
-      <c r="C17" s="124" t="s">
+      <c r="C17" s="112" t="s">
         <v>133</v>
       </c>
-      <c r="D17" s="124" t="s">
+      <c r="D17" s="112" t="s">
         <v>156</v>
       </c>
-      <c r="E17" s="124" t="s">
+      <c r="E17" s="112" t="s">
         <v>156</v>
       </c>
-      <c r="F17" s="124" t="s">
+      <c r="F17" s="112" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="124"/>
-      <c r="H17" s="124"/>
-      <c r="I17" s="124"/>
-      <c r="J17" s="124"/>
+      <c r="G17" s="112"/>
+      <c r="H17" s="112"/>
+      <c r="I17" s="112"/>
+      <c r="J17" s="112"/>
     </row>
     <row r="18" spans="2:10">
-      <c r="C18" s="124" t="s">
+      <c r="C18" s="112" t="s">
         <v>133</v>
       </c>
-      <c r="D18" s="124" t="s">
+      <c r="D18" s="112" t="s">
         <v>157</v>
       </c>
-      <c r="E18" s="124" t="s">
+      <c r="E18" s="112" t="s">
         <v>158</v>
       </c>
-      <c r="F18" s="124" t="s">
+      <c r="F18" s="112" t="s">
         <v>51</v>
       </c>
-      <c r="G18" s="124"/>
-      <c r="H18" s="124"/>
-      <c r="I18" s="124"/>
-      <c r="J18" s="124"/>
+      <c r="G18" s="112"/>
+      <c r="H18" s="112"/>
+      <c r="I18" s="112"/>
+      <c r="J18" s="112"/>
     </row>
     <row r="19" spans="2:10">
-      <c r="C19" s="124" t="s">
+      <c r="C19" s="112" t="s">
         <v>133</v>
       </c>
-      <c r="D19" s="124" t="s">
+      <c r="D19" s="112" t="s">
         <v>159</v>
       </c>
-      <c r="E19" s="124" t="s">
+      <c r="E19" s="112" t="s">
         <v>160</v>
       </c>
-      <c r="F19" s="124" t="s">
+      <c r="F19" s="112" t="s">
         <v>51</v>
       </c>
-      <c r="G19" s="124"/>
-      <c r="H19" s="124"/>
-      <c r="I19" s="124"/>
-      <c r="J19" s="124"/>
+      <c r="G19" s="112"/>
+      <c r="H19" s="112"/>
+      <c r="I19" s="112"/>
+      <c r="J19" s="112"/>
     </row>
     <row r="20" spans="2:10">
-      <c r="C20" s="124" t="s">
+      <c r="C20" s="112" t="s">
         <v>164</v>
       </c>
-      <c r="D20" s="124" t="s">
+      <c r="D20" s="112" t="s">
         <v>161</v>
       </c>
-      <c r="E20" s="124" t="s">
+      <c r="E20" s="112" t="s">
         <v>162</v>
       </c>
-      <c r="F20" s="124" t="s">
+      <c r="F20" s="112" t="s">
         <v>163</v>
       </c>
-      <c r="G20" s="124"/>
-      <c r="H20" s="124"/>
-      <c r="I20" s="124"/>
-      <c r="J20" s="124"/>
+      <c r="G20" s="112"/>
+      <c r="H20" s="112"/>
+      <c r="I20" s="112"/>
+      <c r="J20" s="112"/>
     </row>
     <row r="21" spans="2:10">
       <c r="C21" t="s">
@@ -6663,30 +6550,30 @@
       </c>
     </row>
     <row r="23" spans="2:10">
-      <c r="C23" s="124" t="s">
+      <c r="C23" s="112" t="s">
         <v>164</v>
       </c>
-      <c r="D23" s="124" t="s">
+      <c r="D23" s="112" t="s">
         <v>288</v>
       </c>
-      <c r="E23" s="124" t="s">
+      <c r="E23" s="112" t="s">
         <v>289</v>
       </c>
       <c r="F23" t="s">
         <v>163</v>
       </c>
-      <c r="G23" s="124" t="s">
+      <c r="G23" s="112" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="24" spans="2:10">
-      <c r="C24" s="124" t="s">
+      <c r="C24" s="112" t="s">
         <v>133</v>
       </c>
-      <c r="D24" s="124" t="s">
+      <c r="D24" s="112" t="s">
         <v>176</v>
       </c>
-      <c r="E24" s="124" t="s">
+      <c r="E24" s="112" t="s">
         <v>178</v>
       </c>
       <c r="F24" t="s">
@@ -6694,10 +6581,10 @@
       </c>
     </row>
     <row r="25" spans="2:10">
-      <c r="D25" s="124" t="s">
+      <c r="D25" s="112" t="s">
         <v>177</v>
       </c>
-      <c r="E25" s="124" t="s">
+      <c r="E25" s="112" t="s">
         <v>179</v>
       </c>
       <c r="F25" t="s">
@@ -6708,10 +6595,10 @@
       <c r="C26" t="s">
         <v>164</v>
       </c>
-      <c r="D26" s="124" t="s">
+      <c r="D26" s="112" t="s">
         <v>189</v>
       </c>
-      <c r="E26" s="124" t="s">
+      <c r="E26" s="112" t="s">
         <v>190</v>
       </c>
       <c r="F26" t="s">
@@ -6725,10 +6612,10 @@
       <c r="C27" t="s">
         <v>133</v>
       </c>
-      <c r="D27" s="124" t="s">
+      <c r="D27" s="112" t="s">
         <v>202</v>
       </c>
-      <c r="E27" s="124" t="s">
+      <c r="E27" s="112" t="s">
         <v>204</v>
       </c>
       <c r="F27" t="s">
@@ -6745,10 +6632,10 @@
       <c r="C28" t="s">
         <v>164</v>
       </c>
-      <c r="D28" s="124" t="s">
+      <c r="D28" s="112" t="s">
         <v>202</v>
       </c>
-      <c r="E28" s="124" t="s">
+      <c r="E28" s="112" t="s">
         <v>205</v>
       </c>
       <c r="F28" t="s">
@@ -6760,7 +6647,7 @@
         <f>LEFT(D29,3)</f>
         <v>ENV</v>
       </c>
-      <c r="D29" s="124" t="s">
+      <c r="D29" s="112" t="s">
         <v>206</v>
       </c>
       <c r="E29" t="str">
@@ -6776,7 +6663,7 @@
         <f t="shared" ref="C30:C33" si="0">LEFT(D30,3)</f>
         <v>NRG</v>
       </c>
-      <c r="D30" s="124" t="s">
+      <c r="D30" s="112" t="s">
         <v>207</v>
       </c>
       <c r="E30" t="str">
@@ -6792,7 +6679,7 @@
         <f t="shared" si="0"/>
         <v>MAT</v>
       </c>
-      <c r="D31" s="124" t="s">
+      <c r="D31" s="112" t="s">
         <v>208</v>
       </c>
       <c r="E31" t="str">
@@ -6808,7 +6695,7 @@
         <f t="shared" si="0"/>
         <v>FIN</v>
       </c>
-      <c r="D32" s="124" t="s">
+      <c r="D32" s="112" t="s">
         <v>209</v>
       </c>
       <c r="E32" t="str">
@@ -6824,7 +6711,7 @@
         <f t="shared" si="0"/>
         <v>DEM</v>
       </c>
-      <c r="D33" s="124" t="s">
+      <c r="D33" s="112" t="s">
         <v>210</v>
       </c>
       <c r="E33" t="str">
@@ -6832,6 +6719,20 @@
         <v>DEM commodity to test trade pcg</v>
       </c>
       <c r="F33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6">
+      <c r="C34" t="s">
+        <v>164</v>
+      </c>
+      <c r="D34" s="112" t="s">
+        <v>293</v>
+      </c>
+      <c r="E34" t="s">
+        <v>294</v>
+      </c>
+      <c r="F34" t="s">
         <v>51</v>
       </c>
     </row>
@@ -7140,10 +7041,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:F42"/>
+  <dimension ref="A3:G47"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView topLeftCell="A21" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -7190,138 +7091,142 @@
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="125" t="s">
+      <c r="B12" s="113" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="126" t="s">
+      <c r="C12" s="114" t="s">
         <v>74</v>
       </c>
-      <c r="D12" s="127" t="s">
+      <c r="D12" s="115" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="13" spans="2:5">
-      <c r="B13" s="14">
+      <c r="B13" s="13">
         <v>1</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="13">
         <v>1</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="13">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:5">
-      <c r="B14" s="14">
+      <c r="B14" s="13">
         <v>2</v>
       </c>
-      <c r="C14" s="14">
+      <c r="C14" s="13">
         <v>2</v>
       </c>
-      <c r="D14" s="14">
+      <c r="D14" s="13">
         <v>2</v>
       </c>
     </row>
     <row r="15" spans="2:5">
-      <c r="B15" s="14"/>
-      <c r="C15" s="14">
+      <c r="B15" s="13"/>
+      <c r="C15" s="13">
         <v>5</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="13">
         <v>5</v>
       </c>
     </row>
     <row r="16" spans="2:5">
-      <c r="B16" s="14"/>
-      <c r="C16" s="14">
+      <c r="B16" s="13"/>
+      <c r="C16" s="13">
         <v>5</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="B17" s="14"/>
-      <c r="C17" s="14">
+    <row r="17" spans="1:7">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13">
         <v>5</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14">
+    <row r="18" spans="1:7">
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14">
+    <row r="19" spans="1:7">
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14">
+    <row r="20" spans="1:7">
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14">
+    <row r="21" spans="1:7">
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14">
+    <row r="22" spans="1:7">
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14">
+    <row r="23" spans="1:7">
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
-      <c r="A26" s="129" t="s">
+    <row r="26" spans="1:7">
+      <c r="A26" s="117" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>213</v>
       </c>
-      <c r="B27" s="125" t="str">
+      <c r="B27" s="113" t="str">
         <f>"msy"&amp;MAX(B29:B45)&amp;"-"&amp;COUNT(B29:B45)&amp;"p"</f>
         <v>msy2007-2p</v>
       </c>
-      <c r="C27" s="125" t="str">
+      <c r="C27" s="113" t="str">
         <f t="shared" ref="C27:F27" si="0">"msy"&amp;MAX(C29:C45)&amp;"-"&amp;COUNT(C29:C45)&amp;"p"</f>
         <v>msy2015-5p</v>
       </c>
-      <c r="D27" s="125" t="str">
+      <c r="D27" s="113" t="str">
         <f t="shared" si="0"/>
         <v>msy2050-9p</v>
       </c>
-      <c r="E27" s="125" t="str">
+      <c r="E27" s="113" t="str">
         <f t="shared" si="0"/>
         <v>msy2100-14p</v>
       </c>
-      <c r="F27" s="125" t="str">
+      <c r="F27" s="113" t="str">
         <f t="shared" si="0"/>
         <v>msy2050-6p</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27" s="113" t="str">
+        <f t="shared" ref="G27" si="1">"msy"&amp;MAX(G29:G45)&amp;"-"&amp;COUNT(G29:G45)&amp;"p"</f>
+        <v>msy2048-17p</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>242</v>
       </c>
@@ -7338,223 +7243,306 @@
         <v>2054</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>243</v>
       </c>
-      <c r="B29" s="14">
+      <c r="B29" s="13">
         <v>2005</v>
       </c>
-      <c r="C29" s="14">
+      <c r="C29" s="13">
         <v>2005</v>
       </c>
-      <c r="D29" s="14">
+      <c r="D29" s="13">
         <v>2005</v>
       </c>
-      <c r="E29" s="14">
+      <c r="E29" s="13">
         <f>D29</f>
         <v>2005</v>
       </c>
-      <c r="F29" s="14">
+      <c r="F29" s="13">
         <f>E29</f>
         <v>2005</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29" s="13">
+        <f>F29</f>
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>243</v>
       </c>
-      <c r="B30" s="14">
+      <c r="B30" s="13">
         <v>2007</v>
       </c>
-      <c r="C30" s="14">
+      <c r="C30" s="13">
         <v>2006</v>
       </c>
-      <c r="D30" s="14">
+      <c r="D30" s="13">
         <v>2015</v>
       </c>
-      <c r="E30" s="14">
-        <f t="shared" ref="E30:F31" si="1">D30</f>
+      <c r="E30" s="13">
+        <f t="shared" ref="E30:G31" si="2">D30</f>
         <v>2015</v>
       </c>
-      <c r="F30" s="14">
-        <f t="shared" si="1"/>
+      <c r="F30" s="13">
+        <f t="shared" si="2"/>
         <v>2015</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30" s="13">
+        <f t="shared" si="2"/>
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>243</v>
       </c>
-      <c r="B31" s="14"/>
-      <c r="C31" s="14">
+      <c r="B31" s="13"/>
+      <c r="C31" s="13">
         <v>2007</v>
       </c>
-      <c r="D31" s="14">
+      <c r="D31" s="13">
         <f>D30+5</f>
         <v>2020</v>
       </c>
-      <c r="E31" s="14">
-        <f t="shared" si="1"/>
+      <c r="E31" s="13">
+        <f t="shared" si="2"/>
         <v>2020</v>
       </c>
-      <c r="F31" s="14">
-        <f t="shared" si="1"/>
+      <c r="F31" s="13">
+        <f t="shared" si="2"/>
         <v>2020</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31" s="13">
+        <f t="shared" si="2"/>
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>243</v>
       </c>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14">
+      <c r="B32" s="13"/>
+      <c r="C32" s="13">
         <v>2010</v>
       </c>
-      <c r="D32" s="14">
-        <f t="shared" ref="D32:D37" si="2">D31+5</f>
+      <c r="D32" s="13">
+        <f t="shared" ref="D32:D37" si="3">D31+5</f>
         <v>2025</v>
       </c>
-      <c r="E32" s="14">
+      <c r="E32" s="13">
         <f>E31+5</f>
         <v>2025</v>
       </c>
-      <c r="F32" s="14">
+      <c r="F32" s="13">
         <f>F31+10</f>
         <v>2030</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32" s="13">
+        <f>G31+2</f>
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>243</v>
       </c>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14">
+      <c r="B33" s="13"/>
+      <c r="C33" s="13">
         <v>2015</v>
       </c>
-      <c r="D33" s="14">
-        <f t="shared" si="2"/>
+      <c r="D33" s="13">
+        <f t="shared" si="3"/>
         <v>2030</v>
       </c>
-      <c r="E33" s="14">
-        <f t="shared" ref="E33:E37" si="3">E32+5</f>
+      <c r="E33" s="13">
+        <f t="shared" ref="E33:E37" si="4">E32+5</f>
         <v>2030</v>
       </c>
-      <c r="F33" s="14">
-        <f t="shared" ref="F33:F34" si="4">F32+10</f>
+      <c r="F33" s="13">
+        <f t="shared" ref="F33:F34" si="5">F32+10</f>
         <v>2040</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33" s="13">
+        <f t="shared" ref="G33:G46" si="6">G32+2</f>
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>243</v>
       </c>
-      <c r="B34" s="14"/>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14">
-        <f t="shared" si="2"/>
-        <v>2035</v>
-      </c>
-      <c r="E34" s="14">
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13">
         <f t="shared" si="3"/>
         <v>2035</v>
       </c>
-      <c r="F34" s="14">
+      <c r="E34" s="13">
+        <f t="shared" si="4"/>
+        <v>2035</v>
+      </c>
+      <c r="F34" s="13">
+        <f t="shared" si="5"/>
+        <v>2050</v>
+      </c>
+      <c r="G34" s="13">
+        <f t="shared" si="6"/>
+        <v>2026</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>243</v>
+      </c>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13">
+        <f t="shared" si="3"/>
+        <v>2040</v>
+      </c>
+      <c r="E35" s="13">
+        <f t="shared" si="4"/>
+        <v>2040</v>
+      </c>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13">
+        <f t="shared" si="6"/>
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>243</v>
+      </c>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13">
+        <f t="shared" si="3"/>
+        <v>2045</v>
+      </c>
+      <c r="E36" s="13">
+        <f t="shared" si="4"/>
+        <v>2045</v>
+      </c>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13">
+        <f t="shared" si="6"/>
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" t="s">
+        <v>243</v>
+      </c>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13">
+        <f t="shared" si="3"/>
+        <v>2050</v>
+      </c>
+      <c r="E37" s="13">
         <f t="shared" si="4"/>
         <v>2050</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" t="s">
-        <v>243</v>
-      </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14">
-        <f t="shared" si="2"/>
-        <v>2040</v>
-      </c>
-      <c r="E35" s="14">
-        <f t="shared" si="3"/>
-        <v>2040</v>
-      </c>
-      <c r="F35" s="14"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" t="s">
-        <v>243</v>
-      </c>
-      <c r="B36" s="14"/>
-      <c r="C36" s="14"/>
-      <c r="D36" s="14">
-        <f t="shared" si="2"/>
-        <v>2045</v>
-      </c>
-      <c r="E36" s="14">
-        <f t="shared" si="3"/>
-        <v>2045</v>
-      </c>
-      <c r="F36" s="14"/>
-    </row>
-    <row r="37" spans="1:6">
-      <c r="A37" t="s">
-        <v>243</v>
-      </c>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14">
-        <f t="shared" si="2"/>
-        <v>2050</v>
-      </c>
-      <c r="E37" s="14">
-        <f t="shared" si="3"/>
-        <v>2050</v>
-      </c>
-      <c r="F37" s="14"/>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="F37" s="13"/>
+      <c r="G37" s="13">
+        <f t="shared" si="6"/>
+        <v>2032</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>243</v>
       </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14">
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13">
         <f>E37+10</f>
         <v>2060</v>
       </c>
-      <c r="F38" s="14"/>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="F38" s="13"/>
+      <c r="G38" s="13">
+        <f t="shared" si="6"/>
+        <v>2034</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>243</v>
       </c>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14">
-        <f t="shared" ref="E39:E42" si="5">E38+10</f>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13">
+        <f t="shared" ref="E39:E42" si="7">E38+10</f>
         <v>2070</v>
       </c>
-      <c r="F39" s="14"/>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="E40" s="14">
-        <f t="shared" si="5"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13">
+        <f t="shared" si="6"/>
+        <v>2036</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="E40" s="13">
+        <f t="shared" si="7"/>
         <v>2080</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="E41" s="14">
-        <f t="shared" si="5"/>
+      <c r="G40" s="13">
+        <f t="shared" si="6"/>
+        <v>2038</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="E41" s="13">
+        <f t="shared" si="7"/>
         <v>2090</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="E42" s="14">
-        <f t="shared" si="5"/>
+      <c r="G41" s="13">
+        <f t="shared" si="6"/>
+        <v>2040</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="E42" s="13">
+        <f t="shared" si="7"/>
         <v>2100</v>
       </c>
+      <c r="G42" s="13">
+        <f t="shared" si="6"/>
+        <v>2042</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="G43" s="13">
+        <f t="shared" si="6"/>
+        <v>2044</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="G44" s="13">
+        <f t="shared" si="6"/>
+        <v>2046</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="G45" s="13">
+        <f t="shared" si="6"/>
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="G46" s="13">
+        <f t="shared" si="6"/>
+        <v>2050</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="G47" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -7585,7 +7573,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15">
-      <c r="A1" s="128">
+      <c r="A1" s="116">
         <v>1</v>
       </c>
     </row>
@@ -7634,10 +7622,10 @@
       <c r="C6" t="s">
         <v>75</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="14">
         <v>0</v>
       </c>
       <c r="F6">
@@ -7648,10 +7636,10 @@
       <c r="C7" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="14">
         <v>0</v>
       </c>
       <c r="F7">
@@ -7661,16 +7649,16 @@
     <row r="18" spans="2:4" ht="19.5" customHeight="1"/>
     <row r="19" spans="2:4" ht="15.75" customHeight="1"/>
     <row r="30" spans="2:4" ht="15">
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="18">
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
     </row>
     <row r="33" spans="2:17">
       <c r="B33" s="1" t="s">
@@ -7731,13 +7719,9 @@
       <c r="D35" t="s">
         <v>4</v>
       </c>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6">
+      <c r="G35">
         <v>2222</v>
       </c>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
       <c r="J35" t="s">
         <v>17</v>
       </c>
@@ -7749,13 +7733,9 @@
       <c r="D36" t="s">
         <v>4</v>
       </c>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6">
+      <c r="G36">
         <v>8888</v>
       </c>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
       <c r="J36" t="s">
         <v>17</v>
       </c>
@@ -7829,22 +7809,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="12"/>
-    <col min="2" max="2" width="12.140625" style="12" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" style="12" customWidth="1"/>
-    <col min="4" max="4" width="14" style="12" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="12" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="9.140625" style="11"/>
+    <col min="2" max="2" width="12.140625" style="11" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="14" style="11" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="11" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:8" ht="15">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="5" spans="2:8">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>18</v>
       </c>
     </row>
@@ -7858,49 +7838,45 @@
       <c r="D6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="123" t="s">
+      <c r="E6" s="111" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="123" t="s">
+      <c r="F6" s="111" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="123" t="s">
+      <c r="G6" s="111" t="s">
         <v>73</v>
       </c>
-      <c r="H6" s="122" t="s">
+      <c r="H6" s="110" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="7" spans="2:8">
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="11">
         <v>2005</v>
       </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
     </row>
     <row r="8" spans="2:8" ht="13.5" customHeight="1">
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="11">
         <v>0.05</v>
       </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
     </row>
     <row r="9" spans="2:8" ht="13.5" customHeight="1">
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="11">
         <v>0.9</v>
       </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="12" t="s">
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="11" t="s">
         <v>55</v>
       </c>
     </row>
@@ -7939,519 +7915,500 @@
       <c r="C15"/>
       <c r="D15"/>
       <c r="E15"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
     </row>
     <row r="16" spans="2:8">
       <c r="B16"/>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
     </row>
     <row r="17" spans="2:14">
       <c r="B17"/>
       <c r="C17"/>
       <c r="D17"/>
       <c r="E17"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
     </row>
     <row r="18" spans="2:14">
       <c r="B18"/>
       <c r="C18"/>
       <c r="D18"/>
       <c r="E18"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
     </row>
     <row r="19" spans="2:14">
       <c r="B19"/>
       <c r="C19"/>
       <c r="D19"/>
       <c r="E19"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
     </row>
     <row r="20" spans="2:14">
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
     </row>
     <row r="21" spans="2:14">
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
       <c r="E21"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
     </row>
     <row r="22" spans="2:14">
       <c r="B22"/>
       <c r="C22"/>
       <c r="D22"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
     </row>
     <row r="23" spans="2:14">
       <c r="B23"/>
       <c r="C23"/>
       <c r="D23"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
     </row>
     <row r="24" spans="2:14" ht="18">
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
     </row>
     <row r="25" spans="2:14">
-      <c r="B25" s="23"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
     </row>
     <row r="26" spans="2:14">
-      <c r="B26" s="79" t="s">
+      <c r="B26" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="80" t="s">
+      <c r="C26" s="71" t="s">
         <v>97</v>
       </c>
-      <c r="D26" s="81" t="s">
+      <c r="D26" s="72" t="s">
         <v>98</v>
       </c>
-      <c r="E26" s="81" t="s">
+      <c r="E26" s="72" t="s">
         <v>99</v>
       </c>
-      <c r="F26" s="81" t="s">
+      <c r="F26" s="72" t="s">
         <v>57</v>
       </c>
-      <c r="G26" s="81" t="s">
+      <c r="G26" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="H26" s="81" t="s">
+      <c r="H26" s="72" t="s">
         <v>100</v>
       </c>
-      <c r="I26" s="81" t="s">
+      <c r="I26" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="J26" s="81" t="s">
+      <c r="J26" s="72" t="s">
         <v>102</v>
       </c>
-      <c r="K26" s="81" t="s">
+      <c r="K26" s="72" t="s">
         <v>103</v>
       </c>
-      <c r="L26" s="81" t="s">
+      <c r="L26" s="72" t="s">
         <v>59</v>
       </c>
-      <c r="M26" s="81" t="s">
+      <c r="M26" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="N26" s="82" t="s">
+      <c r="N26" s="73" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="27" spans="2:14">
-      <c r="B27" s="83"/>
-      <c r="C27" s="80" t="s">
+      <c r="B27" s="74"/>
+      <c r="C27" s="71" t="s">
         <v>105</v>
       </c>
-      <c r="D27" s="81" t="s">
+      <c r="D27" s="72" t="s">
         <v>106</v>
       </c>
-      <c r="E27" s="81" t="s">
+      <c r="E27" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="F27" s="81" t="s">
+      <c r="F27" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="G27" s="81" t="s">
+      <c r="G27" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="H27" s="81" t="s">
+      <c r="H27" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="I27" s="81" t="s">
+      <c r="I27" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="J27" s="81" t="s">
+      <c r="J27" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="K27" s="81" t="s">
+      <c r="K27" s="72" t="s">
         <v>111</v>
       </c>
-      <c r="L27" s="81" t="s">
+      <c r="L27" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="M27" s="81" t="s">
+      <c r="M27" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="N27" s="82" t="s">
+      <c r="N27" s="73" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="28" spans="2:14">
-      <c r="B28" s="84" t="s">
+      <c r="B28" s="75" t="s">
         <v>49</v>
       </c>
-      <c r="C28" s="85">
+      <c r="C28" s="76">
         <f>C38/$F38*$D31</f>
         <v>9.417808219178081E-2</v>
       </c>
-      <c r="D28" s="86">
+      <c r="D28" s="77">
         <f>D38/$F38*$D31</f>
         <v>0.10273972602739725</v>
       </c>
-      <c r="E28" s="86">
+      <c r="E28" s="77">
         <f>E38/$F38*$D31</f>
         <v>8.5616438356164379E-3</v>
       </c>
-      <c r="F28" s="86">
+      <c r="F28" s="77">
         <f>C39/$F39*$D32</f>
         <v>0.13835616438356163</v>
       </c>
-      <c r="G28" s="86">
+      <c r="G28" s="77">
         <f>D39/$F39*$D32</f>
         <v>0.12682648401826482</v>
       </c>
-      <c r="H28" s="86">
+      <c r="H28" s="77">
         <f>E39/$F39*$D32</f>
         <v>1.1529680365296802E-2</v>
       </c>
-      <c r="I28" s="86">
+      <c r="I28" s="77">
         <f>C40/$F40*$D33</f>
         <v>9.9200913242009123E-2</v>
       </c>
-      <c r="J28" s="86">
+      <c r="J28" s="77">
         <f>D40/$F40*$D33</f>
         <v>0.10821917808219178</v>
       </c>
-      <c r="K28" s="86">
+      <c r="K28" s="77">
         <f>E40/$F40*$D33</f>
         <v>9.0182648401826472E-3</v>
       </c>
-      <c r="L28" s="86">
+      <c r="L28" s="77">
         <f>C41/$F41*$D34</f>
         <v>0.13812785388127852</v>
       </c>
-      <c r="M28" s="86">
+      <c r="M28" s="77">
         <f>D41/$F41*$D34</f>
         <v>0.15068493150684931</v>
       </c>
-      <c r="N28" s="87">
+      <c r="N28" s="78">
         <f>E41/$F41*$D34</f>
         <v>1.2557077625570776E-2</v>
       </c>
     </row>
     <row r="29" spans="2:14">
-      <c r="B29" s="88"/>
-      <c r="C29" s="88"/>
-      <c r="D29" s="88"/>
-      <c r="E29" s="88"/>
-      <c r="F29" s="88"/>
-      <c r="G29" s="88"/>
-      <c r="H29" s="88"/>
-      <c r="I29" s="89"/>
-      <c r="J29" s="89"/>
-      <c r="K29" s="89"/>
-      <c r="L29" s="89"/>
-      <c r="M29" s="89"/>
-      <c r="N29" s="89"/>
+      <c r="B29" s="79"/>
+      <c r="C29" s="79"/>
+      <c r="D29" s="79"/>
+      <c r="E29" s="79"/>
+      <c r="F29" s="79"/>
+      <c r="G29" s="79"/>
+      <c r="H29" s="79"/>
+      <c r="I29" s="79"/>
+      <c r="J29" s="79"/>
+      <c r="K29" s="79"/>
+      <c r="L29" s="79"/>
+      <c r="M29" s="79"/>
+      <c r="N29" s="79"/>
     </row>
     <row r="30" spans="2:14">
-      <c r="B30" s="90" t="s">
+      <c r="B30" s="80" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="91" t="s">
+      <c r="C30" s="81" t="s">
         <v>66</v>
       </c>
-      <c r="D30" s="92" t="s">
+      <c r="D30" s="82" t="s">
         <v>67</v>
       </c>
-      <c r="E30" s="93" t="s">
+      <c r="E30" s="83" t="s">
         <v>113</v>
       </c>
-      <c r="F30" s="92"/>
-      <c r="G30" s="94"/>
-      <c r="H30" s="94"/>
-      <c r="I30" s="88"/>
-      <c r="J30" s="89"/>
-      <c r="K30" s="89"/>
-      <c r="L30" s="89"/>
-      <c r="M30" s="89"/>
-      <c r="N30" s="89"/>
+      <c r="F30" s="82"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="79"/>
+      <c r="I30" s="79"/>
+      <c r="J30" s="79"/>
+      <c r="K30" s="79"/>
+      <c r="L30" s="79"/>
+      <c r="M30" s="79"/>
+      <c r="N30" s="79"/>
     </row>
     <row r="31" spans="2:14">
-      <c r="B31" s="95" t="s">
+      <c r="B31" s="84" t="s">
         <v>95</v>
       </c>
-      <c r="C31" s="96">
+      <c r="C31" s="85">
         <v>75</v>
       </c>
-      <c r="D31" s="97">
+      <c r="D31" s="86">
         <f>C31/C35</f>
         <v>0.20547945205479451</v>
       </c>
-      <c r="E31" s="98" t="s">
+      <c r="E31" s="87" t="s">
         <v>114</v>
       </c>
-      <c r="F31" s="99"/>
-      <c r="G31" s="94"/>
-      <c r="H31" s="94"/>
-      <c r="I31" s="88"/>
-      <c r="J31" s="89"/>
-      <c r="K31" s="89"/>
-      <c r="L31" s="89"/>
-      <c r="M31" s="89"/>
-      <c r="N31" s="89"/>
+      <c r="F31" s="88"/>
+      <c r="G31" s="79"/>
+      <c r="H31" s="79"/>
+      <c r="I31" s="79"/>
+      <c r="J31" s="79"/>
+      <c r="K31" s="79"/>
+      <c r="L31" s="79"/>
+      <c r="M31" s="79"/>
+      <c r="N31" s="79"/>
     </row>
     <row r="32" spans="2:14">
-      <c r="B32" s="100" t="s">
+      <c r="B32" s="89" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="96">
+      <c r="C32" s="85">
         <v>101</v>
       </c>
-      <c r="D32" s="97">
+      <c r="D32" s="86">
         <f>C32/C35</f>
         <v>0.27671232876712326</v>
       </c>
-      <c r="E32" s="98" t="s">
+      <c r="E32" s="87" t="s">
         <v>115</v>
       </c>
-      <c r="F32" s="99"/>
-      <c r="G32" s="94"/>
-      <c r="H32" s="94"/>
-      <c r="I32" s="88"/>
-      <c r="J32" s="89"/>
-      <c r="K32" s="89"/>
-      <c r="L32" s="89"/>
-      <c r="M32" s="89"/>
-      <c r="N32" s="89"/>
+      <c r="F32" s="88"/>
+      <c r="G32" s="79"/>
+      <c r="H32" s="79"/>
+      <c r="I32" s="79"/>
+      <c r="J32" s="79"/>
+      <c r="K32" s="79"/>
+      <c r="L32" s="79"/>
+      <c r="M32" s="79"/>
+      <c r="N32" s="79"/>
     </row>
     <row r="33" spans="2:14">
-      <c r="B33" s="100" t="s">
+      <c r="B33" s="89" t="s">
         <v>88</v>
       </c>
-      <c r="C33" s="96">
+      <c r="C33" s="85">
         <v>79</v>
       </c>
-      <c r="D33" s="97">
+      <c r="D33" s="86">
         <f>C33/C35</f>
         <v>0.21643835616438356</v>
       </c>
-      <c r="E33" s="98" t="s">
+      <c r="E33" s="87" t="s">
         <v>116</v>
       </c>
-      <c r="F33" s="99"/>
-      <c r="G33" s="94"/>
-      <c r="H33" s="94"/>
-      <c r="I33" s="89"/>
-      <c r="J33" s="89"/>
-      <c r="K33" s="89"/>
-      <c r="L33" s="89"/>
-      <c r="M33" s="89"/>
-      <c r="N33" s="89"/>
+      <c r="F33" s="88"/>
+      <c r="G33" s="79"/>
+      <c r="H33" s="79"/>
+      <c r="I33" s="79"/>
+      <c r="J33" s="79"/>
+      <c r="K33" s="79"/>
+      <c r="L33" s="79"/>
+      <c r="M33" s="79"/>
+      <c r="N33" s="79"/>
     </row>
     <row r="34" spans="2:14">
-      <c r="B34" s="101" t="s">
+      <c r="B34" s="90" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="102">
+      <c r="C34" s="91">
         <v>110</v>
       </c>
-      <c r="D34" s="103">
+      <c r="D34" s="92">
         <f>C34/C35</f>
         <v>0.30136986301369861</v>
       </c>
-      <c r="E34" s="104" t="s">
+      <c r="E34" s="93" t="s">
         <v>117</v>
       </c>
-      <c r="F34" s="105"/>
-      <c r="G34" s="94"/>
-      <c r="H34" s="94"/>
-      <c r="I34" s="89"/>
-      <c r="J34" s="89"/>
-      <c r="K34" s="89"/>
-      <c r="L34" s="89"/>
-      <c r="M34" s="89"/>
-      <c r="N34" s="89"/>
+      <c r="F34" s="94"/>
+      <c r="G34" s="79"/>
+      <c r="H34" s="79"/>
+      <c r="I34" s="79"/>
+      <c r="J34" s="79"/>
+      <c r="K34" s="79"/>
+      <c r="L34" s="79"/>
+      <c r="M34" s="79"/>
+      <c r="N34" s="79"/>
     </row>
     <row r="35" spans="2:14">
-      <c r="B35" s="89"/>
-      <c r="C35" s="106">
+      <c r="B35" s="79"/>
+      <c r="C35" s="95">
         <f>SUM(C31:C34)</f>
         <v>365</v>
       </c>
-      <c r="D35" s="107">
+      <c r="D35" s="96">
         <f>SUM(D31:D34)</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="E35" s="108"/>
-      <c r="F35" s="106"/>
-      <c r="G35" s="94"/>
-      <c r="H35" s="94"/>
-      <c r="I35" s="89"/>
-      <c r="J35" s="89"/>
-      <c r="K35" s="89"/>
-      <c r="L35" s="89"/>
-      <c r="M35" s="89"/>
-      <c r="N35" s="89"/>
+      <c r="E35" s="97"/>
+      <c r="F35" s="95"/>
+      <c r="G35" s="79"/>
+      <c r="H35" s="79"/>
+      <c r="I35" s="79"/>
+      <c r="J35" s="79"/>
+      <c r="K35" s="79"/>
+      <c r="L35" s="79"/>
+      <c r="M35" s="79"/>
+      <c r="N35" s="79"/>
     </row>
     <row r="36" spans="2:14">
-      <c r="B36" s="89"/>
-      <c r="C36" s="94"/>
-      <c r="D36" s="109"/>
-      <c r="E36" s="94"/>
-      <c r="F36" s="94"/>
-      <c r="G36" s="94"/>
-      <c r="H36" s="94"/>
-      <c r="I36" s="89"/>
-      <c r="J36" s="89"/>
-      <c r="K36" s="89"/>
-      <c r="L36" s="89"/>
-      <c r="M36" s="89"/>
-      <c r="N36" s="89"/>
+      <c r="B36" s="79"/>
+      <c r="C36" s="79"/>
+      <c r="D36" s="98"/>
+      <c r="E36" s="79"/>
+      <c r="F36" s="79"/>
+      <c r="G36" s="79"/>
+      <c r="H36" s="79"/>
+      <c r="I36" s="79"/>
+      <c r="J36" s="79"/>
+      <c r="K36" s="79"/>
+      <c r="L36" s="79"/>
+      <c r="M36" s="79"/>
+      <c r="N36" s="79"/>
     </row>
     <row r="37" spans="2:14">
-      <c r="B37" s="90" t="s">
+      <c r="B37" s="80" t="s">
         <v>118</v>
       </c>
-      <c r="C37" s="110" t="s">
+      <c r="C37" s="99" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="111" t="s">
+      <c r="D37" s="100" t="s">
         <v>72</v>
       </c>
-      <c r="E37" s="91" t="s">
+      <c r="E37" s="81" t="s">
         <v>87</v>
       </c>
-      <c r="F37" s="94"/>
-      <c r="G37" s="94"/>
-      <c r="H37" s="94"/>
-      <c r="I37" s="89"/>
-      <c r="J37" s="89"/>
-      <c r="K37" s="89"/>
-      <c r="L37" s="89"/>
-      <c r="M37" s="89"/>
-      <c r="N37" s="89"/>
+      <c r="F37" s="79"/>
+      <c r="G37" s="79"/>
+      <c r="H37" s="79"/>
+      <c r="I37" s="79"/>
+      <c r="J37" s="79"/>
+      <c r="K37" s="79"/>
+      <c r="L37" s="79"/>
+      <c r="M37" s="79"/>
+      <c r="N37" s="79"/>
     </row>
     <row r="38" spans="2:14">
-      <c r="B38" s="112" t="s">
+      <c r="B38" s="101" t="s">
         <v>95</v>
       </c>
-      <c r="C38" s="113">
+      <c r="C38" s="102">
         <v>11</v>
       </c>
-      <c r="D38" s="114">
+      <c r="D38" s="103">
         <v>12</v>
       </c>
-      <c r="E38" s="113">
+      <c r="E38" s="102">
         <v>1</v>
       </c>
-      <c r="F38" s="106">
+      <c r="F38" s="95">
         <f>SUM(C38:E38)</f>
         <v>24</v>
       </c>
-      <c r="G38" s="94"/>
-      <c r="H38" s="94"/>
-      <c r="I38" s="89"/>
-      <c r="J38" s="89"/>
-      <c r="K38" s="89"/>
-      <c r="L38" s="89"/>
-      <c r="M38" s="89"/>
-      <c r="N38" s="89"/>
+      <c r="G38" s="79"/>
+      <c r="H38" s="79"/>
+      <c r="I38" s="79"/>
+      <c r="J38" s="79"/>
+      <c r="K38" s="79"/>
+      <c r="L38" s="79"/>
+      <c r="M38" s="79"/>
+      <c r="N38" s="79"/>
     </row>
     <row r="39" spans="2:14">
-      <c r="B39" s="115" t="s">
+      <c r="B39" s="104" t="s">
         <v>68</v>
       </c>
-      <c r="C39" s="116">
+      <c r="C39" s="105">
         <v>12</v>
       </c>
-      <c r="D39" s="117">
+      <c r="D39" s="106">
         <v>11</v>
       </c>
-      <c r="E39" s="116">
+      <c r="E39" s="105">
         <v>1</v>
       </c>
-      <c r="F39" s="106">
+      <c r="F39" s="95">
         <f>SUM(C39:E39)</f>
         <v>24</v>
       </c>
-      <c r="G39" s="106"/>
-      <c r="H39" s="94"/>
-      <c r="I39" s="89"/>
-      <c r="J39" s="89"/>
-      <c r="K39" s="89"/>
-      <c r="L39" s="89"/>
-      <c r="M39" s="89"/>
-      <c r="N39" s="89"/>
+      <c r="G39" s="95"/>
+      <c r="H39" s="79"/>
+      <c r="I39" s="79"/>
+      <c r="J39" s="79"/>
+      <c r="K39" s="79"/>
+      <c r="L39" s="79"/>
+      <c r="M39" s="79"/>
+      <c r="N39" s="79"/>
     </row>
     <row r="40" spans="2:14">
-      <c r="B40" s="115" t="s">
+      <c r="B40" s="104" t="s">
         <v>88</v>
       </c>
-      <c r="C40" s="116">
+      <c r="C40" s="105">
         <v>11</v>
       </c>
-      <c r="D40" s="117">
+      <c r="D40" s="106">
         <v>12</v>
       </c>
-      <c r="E40" s="116">
+      <c r="E40" s="105">
         <v>1</v>
       </c>
-      <c r="F40" s="118">
+      <c r="F40" s="95">
         <f>SUM(C40:E40)</f>
         <v>24</v>
       </c>
-      <c r="G40" s="118"/>
-      <c r="H40" s="94"/>
-      <c r="I40" s="89"/>
-      <c r="J40" s="89"/>
-      <c r="K40" s="89"/>
-      <c r="L40" s="89"/>
-      <c r="M40" s="89"/>
-      <c r="N40" s="89"/>
+      <c r="G40" s="95"/>
+      <c r="H40" s="79"/>
+      <c r="I40" s="79"/>
+      <c r="J40" s="79"/>
+      <c r="K40" s="79"/>
+      <c r="L40" s="79"/>
+      <c r="M40" s="79"/>
+      <c r="N40" s="79"/>
     </row>
     <row r="41" spans="2:14">
-      <c r="B41" s="119" t="s">
+      <c r="B41" s="107" t="s">
         <v>69</v>
       </c>
-      <c r="C41" s="120">
+      <c r="C41" s="108">
         <v>11</v>
       </c>
-      <c r="D41" s="121">
+      <c r="D41" s="109">
         <v>12</v>
       </c>
-      <c r="E41" s="120">
+      <c r="E41" s="108">
         <v>1</v>
       </c>
-      <c r="F41" s="118">
+      <c r="F41" s="95">
         <f>SUM(C41:E41)</f>
         <v>24</v>
       </c>
-      <c r="G41" s="118"/>
-      <c r="H41" s="94"/>
-      <c r="I41" s="89"/>
-      <c r="J41" s="89"/>
-      <c r="K41" s="89"/>
-      <c r="L41" s="89"/>
-      <c r="M41" s="89"/>
-      <c r="N41" s="89"/>
+      <c r="G41" s="95"/>
+      <c r="H41" s="79"/>
+      <c r="I41" s="79"/>
+      <c r="J41" s="79"/>
+      <c r="K41" s="79"/>
+      <c r="L41" s="79"/>
+      <c r="M41" s="79"/>
+      <c r="N41" s="79"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -8471,475 +8428,436 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="28" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="28" customWidth="1"/>
-    <col min="3" max="3" width="12" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="28" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" style="28" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="12" style="28" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" style="28" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" style="28" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="28"/>
+    <col min="1" max="1" width="2.7109375" style="23" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="12" style="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" style="23" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="12" style="23" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="23" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" style="23" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:14">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="22" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="2:14" ht="13.5" thickBot="1">
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="23" t="s">
         <v>192</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="23" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:14">
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="23" t="s">
         <v>191</v>
       </c>
-      <c r="F4" s="30">
+      <c r="F4" s="25">
         <v>0.8</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="23" t="s">
         <v>188</v>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="23" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="6" spans="2:14">
-      <c r="F6" s="31"/>
+      <c r="F6" s="26"/>
     </row>
     <row r="7" spans="2:14" ht="18">
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="33"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="34"/>
-      <c r="K7" s="34"/>
-      <c r="L7" s="34"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
     </row>
     <row r="8" spans="2:14">
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="34"/>
-      <c r="L8" s="34"/>
-      <c r="M8" s="34"/>
-      <c r="N8" s="34"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
     </row>
     <row r="9" spans="2:14">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="D9" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="E9" s="38" t="s">
+      <c r="E9" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="F9" s="38" t="s">
+      <c r="F9" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="G9" s="38" t="s">
+      <c r="G9" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="H9" s="38" t="s">
+      <c r="H9" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="I9" s="38" t="s">
+      <c r="I9" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="J9" s="38" t="s">
+      <c r="J9" s="33" t="s">
         <v>102</v>
       </c>
-      <c r="K9" s="38" t="s">
+      <c r="K9" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="L9" s="38" t="s">
+      <c r="L9" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="M9" s="38" t="s">
+      <c r="M9" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="N9" s="39" t="s">
+      <c r="N9" s="34" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="10" spans="2:14">
-      <c r="B10" s="40"/>
-      <c r="C10" s="37" t="s">
+      <c r="B10" s="35"/>
+      <c r="C10" s="32" t="s">
         <v>105</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="D10" s="33" t="s">
         <v>106</v>
       </c>
-      <c r="E10" s="38" t="s">
+      <c r="E10" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="F10" s="38" t="s">
+      <c r="F10" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="G10" s="38" t="s">
+      <c r="G10" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="H10" s="38" t="s">
+      <c r="H10" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="I10" s="38" t="s">
+      <c r="I10" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="J10" s="38" t="s">
+      <c r="J10" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="K10" s="38" t="s">
+      <c r="K10" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="L10" s="38" t="s">
+      <c r="L10" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="M10" s="38" t="s">
+      <c r="M10" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="N10" s="39" t="s">
+      <c r="N10" s="34" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="11" spans="2:14">
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="42">
+      <c r="C11" s="37">
         <f>C23/$F23*$D15</f>
         <v>9.417808219178081E-2</v>
       </c>
-      <c r="D11" s="43">
+      <c r="D11" s="38">
         <f>D23/$F23*$D15</f>
         <v>0.10273972602739725</v>
       </c>
-      <c r="E11" s="43">
+      <c r="E11" s="38">
         <f>E23/$F23*$D15</f>
         <v>8.5616438356164379E-3</v>
       </c>
-      <c r="F11" s="43">
+      <c r="F11" s="38">
         <f>C24/$F24*$D16</f>
         <v>0.12682648401826482</v>
       </c>
-      <c r="G11" s="43">
+      <c r="G11" s="38">
         <f>D24/$F24*$D16</f>
         <v>0.13835616438356163</v>
       </c>
-      <c r="H11" s="43">
+      <c r="H11" s="38">
         <f>E24/$F24*$D16</f>
         <v>1.1529680365296802E-2</v>
       </c>
-      <c r="I11" s="43">
+      <c r="I11" s="38">
         <f>C25/$F25*$D17</f>
         <v>9.9200913242009123E-2</v>
       </c>
-      <c r="J11" s="43">
+      <c r="J11" s="38">
         <f>D25/$F25*$D17</f>
         <v>0.10821917808219178</v>
       </c>
-      <c r="K11" s="43">
+      <c r="K11" s="38">
         <f>E25/$F25*$D17</f>
         <v>9.0182648401826472E-3</v>
       </c>
-      <c r="L11" s="43">
+      <c r="L11" s="38">
         <f>C26/$F26*$D18</f>
         <v>0.13812785388127852</v>
       </c>
-      <c r="M11" s="43">
+      <c r="M11" s="38">
         <f>D26/$F26*$D18</f>
         <v>0.15068493150684931</v>
       </c>
-      <c r="N11" s="44">
+      <c r="N11" s="39">
         <f>E26/$F26*$D18</f>
         <v>1.2557077625570776E-2</v>
       </c>
     </row>
     <row r="12" spans="2:14" ht="14.25">
-      <c r="B12" s="45"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
     </row>
     <row r="13" spans="2:14">
-      <c r="B13" s="47"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
     </row>
     <row r="14" spans="2:14" ht="15.75">
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="50" t="s">
+      <c r="D14" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="51" t="s">
+      <c r="E14" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="F14" s="50"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="45"/>
+      <c r="F14" s="43"/>
     </row>
     <row r="15" spans="2:14">
-      <c r="B15" s="53" t="s">
+      <c r="B15" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="C15" s="54">
+      <c r="C15" s="46">
         <v>75</v>
       </c>
-      <c r="D15" s="55">
+      <c r="D15" s="47">
         <f>C15/C19</f>
         <v>0.20547945205479451</v>
       </c>
-      <c r="E15" s="56" t="s">
+      <c r="E15" s="48" t="s">
         <v>114</v>
       </c>
-      <c r="F15" s="57"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="45"/>
+      <c r="F15" s="49"/>
     </row>
     <row r="16" spans="2:14">
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="54">
+      <c r="C16" s="46">
         <v>101</v>
       </c>
-      <c r="D16" s="55">
+      <c r="D16" s="47">
         <f>C16/C19</f>
         <v>0.27671232876712326</v>
       </c>
-      <c r="E16" s="56" t="s">
+      <c r="E16" s="48" t="s">
         <v>115</v>
       </c>
-      <c r="F16" s="57"/>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="45"/>
-    </row>
-    <row r="17" spans="2:8">
-      <c r="B17" s="58" t="s">
+      <c r="F16" s="49"/>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="C17" s="54">
+      <c r="C17" s="46">
         <v>79</v>
       </c>
-      <c r="D17" s="55">
+      <c r="D17" s="47">
         <f>C17/C19</f>
         <v>0.21643835616438356</v>
       </c>
-      <c r="E17" s="56" t="s">
+      <c r="E17" s="48" t="s">
         <v>116</v>
       </c>
-      <c r="F17" s="57"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="52"/>
-    </row>
-    <row r="18" spans="2:8">
-      <c r="B18" s="59" t="s">
+      <c r="F17" s="49"/>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="60">
+      <c r="C18" s="52">
         <v>110</v>
       </c>
-      <c r="D18" s="61">
+      <c r="D18" s="53">
         <f>C18/C19</f>
         <v>0.30136986301369861</v>
       </c>
-      <c r="E18" s="62" t="s">
+      <c r="E18" s="54" t="s">
         <v>117</v>
       </c>
-      <c r="F18" s="63"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="52"/>
-    </row>
-    <row r="19" spans="2:8">
-      <c r="C19" s="64">
+      <c r="F18" s="55"/>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="C19" s="56">
         <f>SUM(C15:C18)</f>
         <v>365</v>
       </c>
-      <c r="D19" s="65">
+      <c r="D19" s="57">
         <f>SUM(D15:D18)</f>
         <v>0.99999999999999989</v>
       </c>
-      <c r="E19" s="66"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="52"/>
-    </row>
-    <row r="20" spans="2:8">
-      <c r="C20" s="52"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="66"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="52"/>
-      <c r="H20" s="52"/>
-    </row>
-    <row r="21" spans="2:8">
-      <c r="C21" s="52"/>
-      <c r="D21" s="67"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="52"/>
-      <c r="G21" s="52"/>
-      <c r="H21" s="52"/>
-    </row>
-    <row r="22" spans="2:8" ht="15.75">
-      <c r="B22" s="48" t="s">
+      <c r="E19" s="58"/>
+      <c r="F19" s="56"/>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="D20" s="57"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="56"/>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="D21" s="59"/>
+    </row>
+    <row r="22" spans="2:7" ht="15.75">
+      <c r="B22" s="41" t="s">
         <v>118</v>
       </c>
-      <c r="C22" s="68" t="s">
+      <c r="C22" s="60" t="s">
         <v>71</v>
       </c>
-      <c r="D22" s="69" t="s">
+      <c r="D22" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="E22" s="49" t="s">
+      <c r="E22" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="F22" s="52"/>
-      <c r="G22" s="52"/>
-      <c r="H22" s="52"/>
-    </row>
-    <row r="23" spans="2:8">
-      <c r="B23" s="70" t="s">
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23" s="62" t="s">
         <v>95</v>
       </c>
-      <c r="C23" s="68">
+      <c r="C23" s="60">
         <v>11</v>
       </c>
-      <c r="D23" s="38">
+      <c r="D23" s="33">
         <v>12</v>
       </c>
-      <c r="E23" s="68">
+      <c r="E23" s="60">
         <v>1</v>
       </c>
-      <c r="F23" s="64">
+      <c r="F23" s="56">
         <f>SUM(C23:E23)</f>
         <v>24</v>
       </c>
-      <c r="G23" s="52"/>
-      <c r="H23" s="52"/>
-    </row>
-    <row r="24" spans="2:8">
-      <c r="B24" s="71" t="s">
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="C24" s="72">
+      <c r="C24" s="64">
         <v>11</v>
       </c>
-      <c r="D24" s="73">
+      <c r="D24" s="65">
         <v>12</v>
       </c>
-      <c r="E24" s="72">
+      <c r="E24" s="64">
         <v>1</v>
       </c>
-      <c r="F24" s="64">
+      <c r="F24" s="56">
         <f>SUM(C24:E24)</f>
         <v>24</v>
       </c>
-      <c r="G24" s="64"/>
-      <c r="H24" s="52"/>
-    </row>
-    <row r="25" spans="2:8">
-      <c r="B25" s="71" t="s">
+      <c r="G24" s="56"/>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="72">
+      <c r="C25" s="64">
         <v>11</v>
       </c>
-      <c r="D25" s="73">
+      <c r="D25" s="65">
         <v>12</v>
       </c>
-      <c r="E25" s="72">
+      <c r="E25" s="64">
         <v>1</v>
       </c>
-      <c r="F25" s="74">
+      <c r="F25" s="56">
         <f>SUM(C25:E25)</f>
         <v>24</v>
       </c>
-      <c r="G25" s="74"/>
-      <c r="H25" s="52"/>
-    </row>
-    <row r="26" spans="2:8">
-      <c r="B26" s="75" t="s">
+      <c r="G25" s="56"/>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="C26" s="76">
+      <c r="C26" s="67">
         <v>11</v>
       </c>
-      <c r="D26" s="77">
+      <c r="D26" s="68">
         <v>12</v>
       </c>
-      <c r="E26" s="76">
+      <c r="E26" s="67">
         <v>1</v>
       </c>
-      <c r="F26" s="74">
+      <c r="F26" s="56">
         <f>SUM(C26:E26)</f>
         <v>24</v>
       </c>
-      <c r="G26" s="74"/>
-      <c r="H26" s="52"/>
-    </row>
-    <row r="27" spans="2:8">
-      <c r="B27" s="78"/>
-      <c r="C27" s="74"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="74"/>
-      <c r="F27" s="74"/>
-      <c r="G27" s="74"/>
-      <c r="H27" s="52"/>
+      <c r="G26" s="56"/>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="B27" s="69"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="56"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8951,7 +8869,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8848E86-A146-4530-A694-2F38523B621A}">
   <dimension ref="B4:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -8961,128 +8879,128 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:5">
-      <c r="B4" s="134"/>
-      <c r="C4" s="136" t="s">
+      <c r="B4" s="120"/>
+      <c r="C4" s="122" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="134"/>
-      <c r="E4" s="134"/>
+      <c r="D4" s="120"/>
+      <c r="E4" s="120"/>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="134"/>
-      <c r="C5" s="135" t="s">
+      <c r="B5" s="120"/>
+      <c r="C5" s="121" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="135" t="s">
+      <c r="D5" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="135" t="s">
+      <c r="E5" s="121" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="134"/>
-      <c r="C6" s="134" t="s">
+      <c r="B6" s="120"/>
+      <c r="C6" s="120" t="s">
         <v>278</v>
       </c>
-      <c r="D6" s="137" t="s">
+      <c r="D6" s="120" t="s">
         <v>279</v>
       </c>
-      <c r="E6" s="134">
+      <c r="E6" s="120">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="2:5">
-      <c r="B7" s="134"/>
-      <c r="C7" s="134" t="s">
+      <c r="B7" s="120"/>
+      <c r="C7" s="120" t="s">
         <v>278</v>
       </c>
-      <c r="D7" s="134" t="s">
+      <c r="D7" s="120" t="s">
         <v>285</v>
       </c>
-      <c r="E7" s="134">
+      <c r="E7" s="120">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:5">
-      <c r="B8" s="134"/>
-      <c r="C8" s="134" t="s">
+      <c r="B8" s="120"/>
+      <c r="C8" s="120" t="s">
         <v>278</v>
       </c>
-      <c r="D8" s="134" t="s">
+      <c r="D8" s="120" t="s">
         <v>280</v>
       </c>
-      <c r="E8" s="134">
+      <c r="E8" s="120">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="134"/>
-      <c r="C9" s="134" t="s">
+      <c r="B9" s="120"/>
+      <c r="C9" s="120" t="s">
         <v>278</v>
       </c>
-      <c r="D9" s="134" t="s">
+      <c r="D9" s="120" t="s">
         <v>281</v>
       </c>
-      <c r="E9" s="134">
+      <c r="E9" s="120">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="134"/>
-      <c r="C10" s="134" t="s">
+      <c r="B10" s="120"/>
+      <c r="C10" s="120" t="s">
         <v>278</v>
       </c>
-      <c r="D10" s="134" t="s">
+      <c r="D10" s="120" t="s">
         <v>282</v>
       </c>
-      <c r="E10" s="134">
+      <c r="E10" s="120">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:5">
-      <c r="B11" s="134"/>
-      <c r="C11" s="134" t="s">
+      <c r="B11" s="120"/>
+      <c r="C11" s="120" t="s">
         <v>278</v>
       </c>
-      <c r="D11" s="134" t="s">
+      <c r="D11" s="120" t="s">
         <v>283</v>
       </c>
-      <c r="E11" s="134">
+      <c r="E11" s="120">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:5">
-      <c r="B12" s="134"/>
-      <c r="C12" s="134" t="s">
+      <c r="B12" s="120"/>
+      <c r="C12" s="120" t="s">
         <v>278</v>
       </c>
-      <c r="D12" s="134" t="s">
+      <c r="D12" s="120" t="s">
         <v>284</v>
       </c>
-      <c r="E12" s="134">
+      <c r="E12" s="120">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:5">
-      <c r="C13" s="134" t="s">
+      <c r="C13" s="120" t="s">
         <v>278</v>
       </c>
-      <c r="D13" s="134" t="s">
+      <c r="D13" s="120" t="s">
         <v>286</v>
       </c>
-      <c r="E13" s="134">
+      <c r="E13" s="120">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:5">
-      <c r="C14" s="139" t="s">
+      <c r="C14" s="120" t="s">
         <v>278</v>
       </c>
-      <c r="D14" s="139" t="s">
+      <c r="D14" s="120" t="s">
         <v>291</v>
       </c>
-      <c r="E14" s="139">
+      <c r="E14" s="120">
         <v>-1</v>
       </c>
     </row>
@@ -9098,16 +9016,16 @@
       </c>
     </row>
     <row r="18" spans="10:10">
-      <c r="J18" s="133"/>
+      <c r="J18" s="11"/>
     </row>
     <row r="19" spans="10:10">
-      <c r="J19" s="134"/>
+      <c r="J19" s="120"/>
     </row>
     <row r="20" spans="10:10">
-      <c r="J20" s="134"/>
+      <c r="J20" s="120"/>
     </row>
     <row r="21" spans="10:10">
-      <c r="J21" s="134"/>
+      <c r="J21" s="120"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9142,76 +9060,75 @@
       </c>
     </row>
     <row r="3" spans="2:11" ht="13.5" thickBot="1">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="16" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="4" spans="2:11">
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="14" t="s">
         <v>86</v>
       </c>
       <c r="D4" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="14" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="5" spans="2:11">
-      <c r="B5" s="6" t="s">
+      <c r="B5" t="s">
         <v>188</v>
       </c>
       <c r="D5" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="14" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="6" spans="2:11">
-      <c r="B6" s="6"/>
       <c r="D6" t="s">
         <v>47</v>
       </c>
@@ -9227,242 +9144,238 @@
       <c r="H6" t="s">
         <v>51</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="I6" s="14" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="2:11">
-      <c r="B7" s="6"/>
-    </row>
     <row r="13" spans="2:11">
-      <c r="B13" s="131" t="s">
+      <c r="B13" t="s">
         <v>239</v>
       </c>
-      <c r="C13" s="131"/>
     </row>
     <row r="14" spans="2:11">
-      <c r="B14" s="131" t="s">
+      <c r="B14" t="s">
         <v>214</v>
       </c>
-      <c r="C14" s="131" t="s">
+      <c r="C14" t="s">
         <v>215</v>
       </c>
-      <c r="D14" s="130" t="s">
+      <c r="D14" s="118" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="15" spans="2:11">
-      <c r="B15" s="131" t="s">
+      <c r="B15" t="s">
         <v>217</v>
       </c>
-      <c r="C15" s="131" t="s">
+      <c r="C15" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="130">
+      <c r="D15" s="118">
         <v>1055.55</v>
       </c>
-      <c r="K15" s="132" t="s">
+      <c r="K15" s="119" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="16" spans="2:11">
-      <c r="B16" s="131" t="s">
+      <c r="B16" t="s">
         <v>218</v>
       </c>
-      <c r="C16" s="131" t="s">
+      <c r="C16" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="130">
+      <c r="D16" s="118">
         <v>3.6</v>
       </c>
     </row>
     <row r="17" spans="2:11">
-      <c r="B17" s="131" t="s">
+      <c r="B17" t="s">
         <v>219</v>
       </c>
-      <c r="C17" s="131" t="s">
+      <c r="C17" t="s">
         <v>220</v>
       </c>
-      <c r="D17" s="130">
+      <c r="D17" s="118">
         <v>1000</v>
       </c>
-      <c r="K17" s="132" t="s">
+      <c r="K17" s="119" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="18" spans="2:11">
-      <c r="B18" s="131" t="s">
+      <c r="B18" t="s">
         <v>221</v>
       </c>
-      <c r="C18" s="131" t="s">
+      <c r="C18" t="s">
         <v>222</v>
       </c>
-      <c r="D18" s="130">
+      <c r="D18" s="118">
         <v>1000</v>
       </c>
     </row>
     <row r="19" spans="2:11">
-      <c r="B19" s="131" t="s">
+      <c r="B19" t="s">
         <v>223</v>
       </c>
-      <c r="C19" s="131" t="s">
+      <c r="C19" t="s">
         <v>51</v>
       </c>
-      <c r="D19" s="130">
+      <c r="D19" s="118">
         <v>1.05555</v>
       </c>
     </row>
     <row r="20" spans="2:11">
-      <c r="B20" s="131" t="s">
+      <c r="B20" t="s">
         <v>224</v>
       </c>
-      <c r="C20" s="131" t="s">
+      <c r="C20" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="130">
+      <c r="D20" s="118">
         <v>4.1868000000000002E-2</v>
       </c>
     </row>
     <row r="21" spans="2:11">
-      <c r="B21" s="131" t="s">
+      <c r="B21" t="s">
         <v>225</v>
       </c>
-      <c r="C21" s="131" t="s">
+      <c r="C21" t="s">
         <v>51</v>
       </c>
-      <c r="D21" s="130">
+      <c r="D21" s="118">
         <v>41.868000000000002</v>
       </c>
     </row>
     <row r="22" spans="2:11">
-      <c r="B22" s="131" t="s">
+      <c r="B22" t="s">
         <v>226</v>
       </c>
-      <c r="C22" s="131" t="s">
+      <c r="C22" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="130">
+      <c r="D22" s="118">
         <v>3.5999999999999999E-3</v>
       </c>
     </row>
     <row r="23" spans="2:11">
-      <c r="B23" s="131" t="s">
+      <c r="B23" t="s">
         <v>227</v>
       </c>
-      <c r="C23" s="131" t="s">
+      <c r="C23" t="s">
         <v>220</v>
       </c>
-      <c r="D23" s="130">
+      <c r="D23" s="118">
         <v>1000000</v>
       </c>
     </row>
     <row r="24" spans="2:11">
-      <c r="B24" s="131" t="s">
+      <c r="B24" t="s">
         <v>228</v>
       </c>
-      <c r="C24" s="131" t="s">
+      <c r="C24" t="s">
         <v>229</v>
       </c>
-      <c r="D24" s="130">
+      <c r="D24" s="118">
         <v>1000</v>
       </c>
     </row>
     <row r="25" spans="2:11">
-      <c r="B25" s="131" t="s">
+      <c r="B25" t="s">
         <v>230</v>
       </c>
-      <c r="C25" s="131" t="s">
+      <c r="C25" t="s">
         <v>231</v>
       </c>
-      <c r="D25" s="130">
+      <c r="D25" s="118">
         <v>0.15384600000000001</v>
       </c>
     </row>
     <row r="26" spans="2:11">
-      <c r="B26" s="131" t="s">
+      <c r="B26" t="s">
         <v>232</v>
       </c>
-      <c r="C26" s="131" t="s">
+      <c r="C26" t="s">
         <v>233</v>
       </c>
-      <c r="D26" s="130">
+      <c r="D26" s="118">
         <v>-1E-3</v>
       </c>
     </row>
     <row r="27" spans="2:11">
-      <c r="B27" s="131" t="s">
+      <c r="B27" t="s">
         <v>234</v>
       </c>
-      <c r="C27" s="131" t="s">
+      <c r="C27" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="130">
+      <c r="D27" s="118">
         <v>1000</v>
       </c>
     </row>
     <row r="28" spans="2:11">
-      <c r="B28" s="131" t="s">
+      <c r="B28" t="s">
         <v>235</v>
       </c>
-      <c r="C28" s="131" t="s">
+      <c r="C28" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="130">
+      <c r="D28" s="118">
         <v>37.681199999999997</v>
       </c>
     </row>
     <row r="29" spans="2:11">
-      <c r="B29" s="131" t="s">
+      <c r="B29" t="s">
         <v>236</v>
       </c>
-      <c r="C29" s="131" t="s">
+      <c r="C29" t="s">
         <v>51</v>
       </c>
-      <c r="D29" s="130">
+      <c r="D29" s="118">
         <v>2299</v>
       </c>
     </row>
     <row r="30" spans="2:11">
-      <c r="B30" s="131" t="s">
+      <c r="B30" t="s">
         <v>237</v>
       </c>
-      <c r="C30" s="131" t="s">
+      <c r="C30" t="s">
         <v>231</v>
       </c>
-      <c r="D30" s="130">
+      <c r="D30" s="118">
         <v>2.7777769999999999</v>
       </c>
     </row>
     <row r="31" spans="2:11">
-      <c r="B31" s="131" t="s">
+      <c r="B31" t="s">
         <v>238</v>
       </c>
-      <c r="C31" s="131" t="s">
+      <c r="C31" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="130">
+      <c r="D31" s="118">
         <v>3.6</v>
       </c>
     </row>
     <row r="32" spans="2:11">
-      <c r="B32" s="131" t="s">
+      <c r="B32" t="s">
         <v>51</v>
       </c>
-      <c r="C32" s="131" t="s">
+      <c r="C32" t="s">
         <v>51</v>
       </c>
-      <c r="D32" s="130">
+      <c r="D32" s="118">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="2:4">
-      <c r="B33" s="131" t="s">
+      <c r="B33" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="131" t="s">
+      <c r="C33" t="s">
         <v>287</v>
       </c>
-      <c r="D33" s="130">
+      <c r="D33" s="118">
         <v>1000</v>
       </c>
     </row>

</xml_diff>

<commit_message>
removing contents from other_indexes after distributing has broken UPD/MIG of parameters that use other_indexes. Here are cases to test IRE_FLOSUM in browse. SysSettings and QC3 show up with '-' in import_export field.
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\Model_Demo_Adv_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8E95C7-52AA-4DE1-8A22-0980FC05D0B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C2BC98-F747-4211-AD6C-20B2066BB1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28065" yWindow="2475" windowWidth="21600" windowHeight="11333" tabRatio="853" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2573" yWindow="2573" windowWidth="21600" windowHeight="12682" tabRatio="853" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region-Time Slices" sheetId="16" r:id="rId1"/>
@@ -265,7 +265,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="299">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -1159,6 +1159,9 @@
   </si>
   <si>
     <t>ELCTEGAS00</t>
+  </si>
+  <si>
+    <t>IRE_FLOSUM</t>
   </si>
 </sst>
 </file>
@@ -5816,7 +5819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -7534,8 +7537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -7620,6 +7623,17 @@
         <v>0</v>
       </c>
       <c r="F7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="D8" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="E8" s="14">
+        <v>0</v>
+      </c>
+      <c r="F8">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New DINS-AT case; Need start from scratch after creating a timeslices table in SysSettings?
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\Model_Demo_Adv_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C2BC98-F747-4211-AD6C-20B2066BB1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAB2579-CCEA-49D4-AD85-E13101152694}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2573" yWindow="2573" windowWidth="21600" windowHeight="12682" tabRatio="853" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2145" yWindow="2145" windowWidth="21600" windowHeight="12683" tabRatio="853" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region-Time Slices" sheetId="16" r:id="rId1"/>
@@ -265,7 +265,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="300">
   <si>
     <t>~TFM_UPD</t>
   </si>
@@ -1162,6 +1162,9 @@
   </si>
   <si>
     <t>IRE_FLOSUM</t>
+  </si>
+  <si>
+    <t>~TimeSlices</t>
   </si>
 </sst>
 </file>
@@ -5819,8 +5822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:N17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5846,7 +5849,9 @@
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>299</v>
+      </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
@@ -7537,7 +7542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
creating a new case for testing
Topology records not generated from FI_T *when commodities are comma-separated* AND there is no associated attribute.
</commit_message>
<xml_diff>
--- a/SysSettings.xlsx
+++ b/SysSettings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\Model_Demo_Adv_Veda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Veda\Veda\Veda_models\Model_Demo_Adv_Veda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC1619F2-FEDD-4090-8BDC-1A2B4BC4F366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30F72AE-52B3-4385-B27B-4801ABB6EFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" tabRatio="853" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="11423" tabRatio="853" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region-Time Slices" sheetId="16" r:id="rId1"/>
@@ -31,6 +31,32 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Defaults!$B$14:$D$32</definedName>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
+    <definedName name="IQ_CH">110000</definedName>
+    <definedName name="IQ_CQ">5000</definedName>
+    <definedName name="IQ_CY">10000</definedName>
+    <definedName name="IQ_DAILY">500000</definedName>
+    <definedName name="IQ_FH">100000</definedName>
+    <definedName name="IQ_FQ">500</definedName>
+    <definedName name="IQ_FWD_CY" hidden="1">10001</definedName>
+    <definedName name="IQ_FWD_CY1" hidden="1">10002</definedName>
+    <definedName name="IQ_FWD_CY2" hidden="1">10003</definedName>
+    <definedName name="IQ_FWD_FY" hidden="1">1001</definedName>
+    <definedName name="IQ_FWD_FY1" hidden="1">1002</definedName>
+    <definedName name="IQ_FWD_FY2" hidden="1">1003</definedName>
+    <definedName name="IQ_FWD_Q" hidden="1">501</definedName>
+    <definedName name="IQ_FWD_Q1" hidden="1">502</definedName>
+    <definedName name="IQ_FWD_Q2" hidden="1">503</definedName>
+    <definedName name="IQ_FY">1000</definedName>
+    <definedName name="IQ_LATESTK" hidden="1">1000</definedName>
+    <definedName name="IQ_LATESTQ" hidden="1">500</definedName>
+    <definedName name="IQ_LTM">2000</definedName>
+    <definedName name="IQ_LTMMONTH" hidden="1">120000</definedName>
+    <definedName name="IQ_MONTH">15000</definedName>
+    <definedName name="IQ_NTM">6000</definedName>
+    <definedName name="IQ_TODAY" hidden="1">0</definedName>
+    <definedName name="IQ_WEEK">50000</definedName>
+    <definedName name="IQ_YTD">3000</definedName>
+    <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -852,9 +878,6 @@
     <t>NRGO</t>
   </si>
   <si>
-    <t>ELCSOL,ELCWIN</t>
-  </si>
-  <si>
     <t>ExtREG1</t>
   </si>
   <si>
@@ -1255,6 +1278,9 @@
   </si>
   <si>
     <t>~md_dimensions</t>
+  </si>
+  <si>
+    <t>ELCWIN</t>
   </si>
 </sst>
 </file>
@@ -5637,9 +5663,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5677,9 +5703,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5712,9 +5738,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5747,9 +5790,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5940,12 +6000,12 @@
   <sheetData>
     <row r="1" spans="2:14">
       <c r="N1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="2:14">
       <c r="N2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="2:14" ht="13.15">
@@ -5953,7 +6013,7 @@
         <v>10</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -6081,20 +6141,20 @@
     </row>
     <row r="15" spans="2:14">
       <c r="B15" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="16" spans="2:14">
       <c r="C16" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="3:3">
       <c r="C17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -6196,36 +6256,36 @@
     </row>
     <row r="8" spans="2:9">
       <c r="B8" t="s">
+        <v>193</v>
+      </c>
+      <c r="C8" t="s">
         <v>194</v>
       </c>
-      <c r="C8" t="s">
+      <c r="E8" t="s">
+        <v>198</v>
+      </c>
+      <c r="H8" t="s">
         <v>195</v>
       </c>
-      <c r="E8" t="s">
-        <v>199</v>
-      </c>
-      <c r="H8" t="s">
-        <v>196</v>
-      </c>
       <c r="I8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="2:9">
       <c r="B9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C9" t="s">
+        <v>194</v>
+      </c>
+      <c r="E9" t="s">
+        <v>196</v>
+      </c>
+      <c r="H9" t="s">
         <v>195</v>
       </c>
-      <c r="E9" t="s">
-        <v>197</v>
-      </c>
-      <c r="H9" t="s">
-        <v>196</v>
-      </c>
       <c r="I9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="2:9">
@@ -6642,16 +6702,16 @@
         <v>164</v>
       </c>
       <c r="D23" s="112" t="s">
+        <v>287</v>
+      </c>
+      <c r="E23" s="112" t="s">
         <v>288</v>
-      </c>
-      <c r="E23" s="112" t="s">
-        <v>289</v>
       </c>
       <c r="F23" t="s">
         <v>163</v>
       </c>
       <c r="G23" s="112" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="24" spans="2:10">
@@ -6684,10 +6744,10 @@
         <v>164</v>
       </c>
       <c r="D26" s="112" t="s">
+        <v>188</v>
+      </c>
+      <c r="E26" s="112" t="s">
         <v>189</v>
-      </c>
-      <c r="E26" s="112" t="s">
-        <v>190</v>
       </c>
       <c r="F26" t="s">
         <v>51</v>
@@ -6695,36 +6755,36 @@
     </row>
     <row r="27" spans="2:10">
       <c r="B27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C27" t="s">
         <v>133</v>
       </c>
       <c r="D27" s="112" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E27" s="112" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F27" t="s">
         <v>51</v>
       </c>
       <c r="H27" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="28" spans="2:10">
       <c r="B28" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C28" t="s">
         <v>164</v>
       </c>
       <c r="D28" s="112" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E28" s="112" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F28" t="s">
         <v>163</v>
@@ -6736,7 +6796,7 @@
         <v>ENV</v>
       </c>
       <c r="D29" s="112" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E29" t="str">
         <f>C29&amp;" commodity to test trade pcg"</f>
@@ -6752,7 +6812,7 @@
         <v>NRG</v>
       </c>
       <c r="D30" s="112" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" ref="E30:E33" si="1">C30&amp;" commodity to test trade pcg"</f>
@@ -6768,7 +6828,7 @@
         <v>MAT</v>
       </c>
       <c r="D31" s="112" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="1"/>
@@ -6784,14 +6844,14 @@
         <v>FIN</v>
       </c>
       <c r="D32" s="112" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="1"/>
         <v>FIN commodity to test trade pcg</v>
       </c>
       <c r="F32" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="33" spans="3:6">
@@ -6800,7 +6860,7 @@
         <v>DEM</v>
       </c>
       <c r="D33" s="112" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="1"/>
@@ -6815,10 +6875,10 @@
         <v>164</v>
       </c>
       <c r="D34" s="112" t="s">
+        <v>292</v>
+      </c>
+      <c r="E34" t="s">
         <v>293</v>
-      </c>
-      <c r="E34" t="s">
-        <v>294</v>
       </c>
       <c r="F34" t="s">
         <v>51</v>
@@ -6848,7 +6908,7 @@
   <sheetData>
     <row r="2" spans="2:6">
       <c r="B2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="2:6">
@@ -6862,10 +6922,10 @@
         <v>14</v>
       </c>
       <c r="E3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F3" t="s">
         <v>245</v>
-      </c>
-      <c r="F3" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="4" spans="2:6">
@@ -6873,16 +6933,16 @@
         <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D4" t="s">
         <v>72</v>
       </c>
       <c r="E4" t="s">
+        <v>247</v>
+      </c>
+      <c r="F4" t="s">
         <v>248</v>
-      </c>
-      <c r="F4" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="5" spans="2:6">
@@ -6890,16 +6950,16 @@
         <v>88</v>
       </c>
       <c r="C5" t="s">
+        <v>249</v>
+      </c>
+      <c r="D5" t="s">
         <v>250</v>
       </c>
-      <c r="D5" t="s">
-        <v>251</v>
-      </c>
       <c r="E5" t="s">
+        <v>247</v>
+      </c>
+      <c r="F5" t="s">
         <v>248</v>
-      </c>
-      <c r="F5" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="6" spans="2:6">
@@ -6907,7 +6967,7 @@
         <v>70</v>
       </c>
       <c r="C6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D6" t="s">
         <v>71</v>
@@ -6916,7 +6976,7 @@
         <v>68</v>
       </c>
       <c r="F6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="2:6">
@@ -6924,202 +6984,202 @@
         <v>95</v>
       </c>
       <c r="D7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="2:6">
       <c r="D8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="9" spans="2:6">
       <c r="D9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="10" spans="2:6">
       <c r="D10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F10" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="2:6">
       <c r="D11" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F11" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="2:6">
       <c r="D12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F12" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="13" spans="2:6">
       <c r="D13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="14" spans="2:6">
       <c r="D14" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F14" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="15" spans="2:6">
       <c r="D15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="16" spans="2:6">
       <c r="D16" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="17" spans="4:6">
       <c r="D17" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F17" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18" spans="4:6">
       <c r="D18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="19" spans="4:6">
       <c r="D19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F19" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="20" spans="4:6">
       <c r="D20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="21" spans="4:6">
       <c r="D21" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F21" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="22" spans="4:6">
       <c r="D22" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F22" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="23" spans="4:6">
       <c r="D23" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F23" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="24" spans="4:6">
       <c r="D24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F24" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="25" spans="4:6">
       <c r="D25" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F25" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26" spans="4:6">
       <c r="D26" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F26" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="27" spans="4:6">
       <c r="D27" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F27" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="28" spans="4:6">
       <c r="D28" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F28" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="29" spans="4:6">
       <c r="D29" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F29" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="30" spans="4:6">
       <c r="D30" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F30" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="31" spans="4:6">
       <c r="D31" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F31" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>
@@ -7151,7 +7211,7 @@
         <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="2:5">
@@ -7282,12 +7342,12 @@
     </row>
     <row r="26" spans="1:7" ht="13.15">
       <c r="A26" s="117" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B27" s="113" t="str">
         <f>"msy"&amp;MAX(B29:B45)&amp;"-"&amp;COUNT(B29:B45)&amp;"p"</f>
@@ -7316,7 +7376,7 @@
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B28">
         <f>MAX(B29:B39)+4</f>
@@ -7333,7 +7393,7 @@
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B29" s="13">
         <v>2005</v>
@@ -7359,7 +7419,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B30" s="13">
         <v>2007</v>
@@ -7385,7 +7445,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B31" s="13"/>
       <c r="C31" s="13">
@@ -7410,7 +7470,7 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B32" s="13"/>
       <c r="C32" s="13">
@@ -7435,7 +7495,7 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B33" s="13"/>
       <c r="C33" s="13">
@@ -7460,7 +7520,7 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -7483,7 +7543,7 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
@@ -7503,7 +7563,7 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
@@ -7523,7 +7583,7 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
@@ -7543,7 +7603,7 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
@@ -7560,7 +7620,7 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
@@ -7736,7 +7796,7 @@
     </row>
     <row r="8" spans="1:7">
       <c r="D8" s="14" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E8" s="14">
         <v>0</v>
@@ -7844,7 +7904,7 @@
     </row>
     <row r="39" spans="2:17" ht="13.15">
       <c r="B39" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="40" spans="2:17" ht="13.15" thickBot="1">
@@ -7893,7 +7953,7 @@
         <v>55</v>
       </c>
       <c r="K41" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="42" spans="2:17">
@@ -7904,7 +7964,7 @@
         <v>55</v>
       </c>
       <c r="K42" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -7921,7 +7981,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="C6:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
@@ -7954,7 +8016,7 @@
         <v>180</v>
       </c>
       <c r="D8" t="s">
-        <v>183</v>
+        <v>317</v>
       </c>
       <c r="E8" t="s">
         <v>182</v>
@@ -8588,7 +8650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B2:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="12.75"/>
   <cols>
@@ -8628,7 +8690,7 @@
         <v>2</v>
       </c>
       <c r="G3" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H3" s="23" t="s">
         <v>3</v>
@@ -8636,13 +8698,13 @@
     </row>
     <row r="4" spans="2:14">
       <c r="D4" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F4" s="25">
         <v>0.8</v>
       </c>
       <c r="G4" s="23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H4" s="23" t="s">
         <v>86</v>
@@ -9066,10 +9128,10 @@
     <row r="6" spans="2:5">
       <c r="B6" s="120"/>
       <c r="C6" s="120" t="s">
+        <v>277</v>
+      </c>
+      <c r="D6" s="120" t="s">
         <v>278</v>
-      </c>
-      <c r="D6" s="120" t="s">
-        <v>279</v>
       </c>
       <c r="E6" s="120">
         <v>1</v>
@@ -9078,10 +9140,10 @@
     <row r="7" spans="2:5">
       <c r="B7" s="120"/>
       <c r="C7" s="120" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D7" s="120" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E7" s="120">
         <v>1</v>
@@ -9090,10 +9152,10 @@
     <row r="8" spans="2:5">
       <c r="B8" s="120"/>
       <c r="C8" s="120" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D8" s="120" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E8" s="120">
         <v>1</v>
@@ -9102,10 +9164,10 @@
     <row r="9" spans="2:5">
       <c r="B9" s="120"/>
       <c r="C9" s="120" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D9" s="120" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E9" s="120">
         <v>1</v>
@@ -9114,10 +9176,10 @@
     <row r="10" spans="2:5">
       <c r="B10" s="120"/>
       <c r="C10" s="120" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D10" s="120" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E10" s="120">
         <v>0</v>
@@ -9126,10 +9188,10 @@
     <row r="11" spans="2:5">
       <c r="B11" s="120"/>
       <c r="C11" s="120" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D11" s="120" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E11" s="120">
         <v>1</v>
@@ -9138,10 +9200,10 @@
     <row r="12" spans="2:5">
       <c r="B12" s="120"/>
       <c r="C12" s="120" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D12" s="120" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E12" s="120">
         <v>1</v>
@@ -9149,10 +9211,10 @@
     </row>
     <row r="13" spans="2:5">
       <c r="C13" s="120" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D13" s="120" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E13" s="120">
         <v>1</v>
@@ -9160,10 +9222,10 @@
     </row>
     <row r="14" spans="2:5">
       <c r="C14" s="120" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D14" s="120" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E14" s="120">
         <v>-1</v>
@@ -9171,10 +9233,10 @@
     </row>
     <row r="15" spans="2:5">
       <c r="C15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D15" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -9188,89 +9250,89 @@
     </row>
     <row r="20" spans="3:10">
       <c r="C20" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="J20" s="120"/>
     </row>
     <row r="21" spans="3:10">
       <c r="C21" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J21" s="120"/>
     </row>
     <row r="22" spans="3:10">
       <c r="C22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="23" spans="3:10">
       <c r="C23" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="24" spans="3:10">
       <c r="C24" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="25" spans="3:10" ht="13.15">
       <c r="C25" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="29" spans="3:10">
       <c r="C29" s="14" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="30" spans="3:10">
       <c r="C30" s="14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D30" s="14" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="31" spans="3:10">
       <c r="C31" s="14" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D31" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="32" spans="3:10">
       <c r="C32" s="14" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="33" spans="3:5">
       <c r="C33" s="14" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E33" s="119" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>
@@ -9355,7 +9417,7 @@
     </row>
     <row r="5" spans="2:11">
       <c r="B5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D5" t="s">
         <v>46</v>
@@ -9398,23 +9460,23 @@
     </row>
     <row r="13" spans="2:11">
       <c r="B13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="2:11">
       <c r="B14" t="s">
+        <v>213</v>
+      </c>
+      <c r="C14" t="s">
         <v>214</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" s="118" t="s">
         <v>215</v>
-      </c>
-      <c r="D14" s="118" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="15" spans="2:11">
       <c r="B15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C15" t="s">
         <v>51</v>
@@ -9423,12 +9485,12 @@
         <v>1055.55</v>
       </c>
       <c r="K15" s="119" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="16" spans="2:11">
       <c r="B16" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C16" t="s">
         <v>51</v>
@@ -9439,24 +9501,24 @@
     </row>
     <row r="17" spans="2:11">
       <c r="B17" t="s">
+        <v>218</v>
+      </c>
+      <c r="C17" t="s">
         <v>219</v>
-      </c>
-      <c r="C17" t="s">
-        <v>220</v>
       </c>
       <c r="D17" s="118">
         <v>1000</v>
       </c>
       <c r="K17" s="119" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="18" spans="2:11">
       <c r="B18" t="s">
+        <v>220</v>
+      </c>
+      <c r="C18" t="s">
         <v>221</v>
-      </c>
-      <c r="C18" t="s">
-        <v>222</v>
       </c>
       <c r="D18" s="118">
         <v>1000</v>
@@ -9464,7 +9526,7 @@
     </row>
     <row r="19" spans="2:11">
       <c r="B19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C19" t="s">
         <v>51</v>
@@ -9475,7 +9537,7 @@
     </row>
     <row r="20" spans="2:11">
       <c r="B20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C20" t="s">
         <v>51</v>
@@ -9486,7 +9548,7 @@
     </row>
     <row r="21" spans="2:11">
       <c r="B21" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C21" t="s">
         <v>51</v>
@@ -9497,7 +9559,7 @@
     </row>
     <row r="22" spans="2:11">
       <c r="B22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C22" t="s">
         <v>51</v>
@@ -9508,10 +9570,10 @@
     </row>
     <row r="23" spans="2:11">
       <c r="B23" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D23" s="118">
         <v>1000000</v>
@@ -9519,10 +9581,10 @@
     </row>
     <row r="24" spans="2:11">
       <c r="B24" t="s">
+        <v>227</v>
+      </c>
+      <c r="C24" t="s">
         <v>228</v>
-      </c>
-      <c r="C24" t="s">
-        <v>229</v>
       </c>
       <c r="D24" s="118">
         <v>1000</v>
@@ -9530,10 +9592,10 @@
     </row>
     <row r="25" spans="2:11">
       <c r="B25" t="s">
+        <v>229</v>
+      </c>
+      <c r="C25" t="s">
         <v>230</v>
-      </c>
-      <c r="C25" t="s">
-        <v>231</v>
       </c>
       <c r="D25" s="118">
         <v>0.15384600000000001</v>
@@ -9541,10 +9603,10 @@
     </row>
     <row r="26" spans="2:11">
       <c r="B26" t="s">
+        <v>231</v>
+      </c>
+      <c r="C26" t="s">
         <v>232</v>
-      </c>
-      <c r="C26" t="s">
-        <v>233</v>
       </c>
       <c r="D26" s="118">
         <v>-1E-3</v>
@@ -9552,7 +9614,7 @@
     </row>
     <row r="27" spans="2:11">
       <c r="B27" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C27" t="s">
         <v>51</v>
@@ -9563,7 +9625,7 @@
     </row>
     <row r="28" spans="2:11">
       <c r="B28" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C28" t="s">
         <v>51</v>
@@ -9574,7 +9636,7 @@
     </row>
     <row r="29" spans="2:11">
       <c r="B29" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C29" t="s">
         <v>51</v>
@@ -9585,10 +9647,10 @@
     </row>
     <row r="30" spans="2:11">
       <c r="B30" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C30" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D30" s="118">
         <v>2.7777769999999999</v>
@@ -9596,7 +9658,7 @@
     </row>
     <row r="31" spans="2:11">
       <c r="B31" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C31" t="s">
         <v>51</v>
@@ -9621,7 +9683,7 @@
         <v>80</v>
       </c>
       <c r="C33" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D33" s="118">
         <v>1000</v>

</xml_diff>